<commit_message>
Added tab with hydrophobicity scales in excel document
</commit_message>
<xml_diff>
--- a/encoding_schemes.xlsx
+++ b/encoding_schemes.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxc533/Documents/Arbejde/PhD/Kurser/Kursusmapper/Algorithms_in_Bioinformatics/Exercises/Algo/Algo2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67189EF-8187-F14A-BF0B-C47C8211E72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD66B6E5-37F9-734C-9EBB-CEB2B1B22B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19440" activeTab="3" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="4" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOSUM50" sheetId="1" r:id="rId1"/>
     <sheet name="ONE_HOT" sheetId="2" r:id="rId2"/>
     <sheet name="ONE_HOT_MOD" sheetId="3" r:id="rId3"/>
     <sheet name="ONE_HOT_FRAC" sheetId="4" r:id="rId4"/>
+    <sheet name="Hydrophobicity scales" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="29">
   <si>
     <t>A</t>
   </si>
@@ -110,12 +112,27 @@
   <si>
     <t>*</t>
   </si>
+  <si>
+    <t>kdHydrophobicitya</t>
+  </si>
+  <si>
+    <t>wwHydrophobicityb</t>
+  </si>
+  <si>
+    <t>hhHydrophobicityc</t>
+  </si>
+  <si>
+    <t>mfHydrophobicityd</t>
+  </si>
+  <si>
+    <t>ttHydrophobicitye</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +143,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,14 +181,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7433,8 +7471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E32605-992C-CA45-B433-1F6AC8D37928}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9941,4 +9979,458 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112F557F-3160-E940-BC16-A2D36F354CDD}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-0.6</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-1.56</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>-0.31</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-0.78</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-1.81</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>-0.32</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-0.13</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="F6" s="4">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="D7" s="4">
+        <v>-0.1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-0.76</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="C8" s="4">
+        <v>-0.17</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>-0.4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>-0.01</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.72</v>
+      </c>
+      <c r="F9" s="4">
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4">
+        <v>-0.7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.78</v>
+      </c>
+      <c r="F10" s="4">
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4">
+        <v>-0.8</v>
+      </c>
+      <c r="C11" s="4">
+        <v>-0.13</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.83</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4">
+        <v>-0.9</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.85</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>-0.38</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4">
+        <v>-1.3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.94</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>-1.6</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-0.45</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2.23</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-1.52</v>
+      </c>
+      <c r="F14" s="4">
+        <v>-1.44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4">
+        <v>-3.2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>-0.96</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2.06</v>
+      </c>
+      <c r="E15" s="4">
+        <v>4.76</v>
+      </c>
+      <c r="F15" s="4">
+        <v>-1.44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>-3.5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>-2.02</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.68</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.64</v>
+      </c>
+      <c r="F16" s="4">
+        <v>-2.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4">
+        <v>-3.5</v>
+      </c>
+      <c r="C17" s="4">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.36</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3.01</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-1.84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="4">
+        <v>-3.5</v>
+      </c>
+      <c r="C18" s="4">
+        <v>-1.23</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3.49</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2.95</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-3.27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4">
+        <v>-3.5</v>
+      </c>
+      <c r="C19" s="4">
+        <v>-0.42</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3.47</v>
+      </c>
+      <c r="F19" s="4">
+        <v>-1.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="4">
+        <v>-3.9</v>
+      </c>
+      <c r="C20" s="4">
+        <v>-0.99</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2.71</v>
+      </c>
+      <c r="E20" s="4">
+        <v>5.39</v>
+      </c>
+      <c r="F20" s="4">
+        <v>-3.46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4">
+        <v>-4.5</v>
+      </c>
+      <c r="C21" s="4">
+        <v>-0.81</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2.58</v>
+      </c>
+      <c r="E21" s="4">
+        <v>3.71</v>
+      </c>
+      <c r="F21" s="4">
+        <v>-2.57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2B67AE-E669-F14D-8707-680391081833}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed 'blosum_file' to 'scheme_file'. Added new encoding scheme 'HYDROP_WWIHS'
</commit_message>
<xml_diff>
--- a/encoding_schemes.xlsx
+++ b/encoding_schemes.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxc533/Documents/Arbejde/PhD/Kurser/Kursusmapper/Algorithms_in_Bioinformatics/Exercises/Algo/Algo2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD66B6E5-37F9-734C-9EBB-CEB2B1B22B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A209F3D1-6178-B64B-80A8-7C3673099DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="4" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOSUM50" sheetId="1" r:id="rId1"/>
     <sheet name="ONE_HOT" sheetId="2" r:id="rId2"/>
     <sheet name="ONE_HOT_MOD" sheetId="3" r:id="rId3"/>
     <sheet name="ONE_HOT_FRAC" sheetId="4" r:id="rId4"/>
-    <sheet name="Hydrophobicity scales" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="HYDROP_WWIHS" sheetId="6" r:id="rId5"/>
+    <sheet name="Hydrophobicity scales" sheetId="5" r:id="rId6"/>
+    <sheet name="Charge" sheetId="7" r:id="rId7"/>
+    <sheet name="Size" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="37">
   <si>
     <t>A</t>
   </si>
@@ -113,19 +115,43 @@
     <t>*</t>
   </si>
   <si>
-    <t>kdHydrophobicitya</t>
+    <t>kdHydrophobicity</t>
   </si>
   <si>
-    <t>wwHydrophobicityb</t>
+    <t>wwHydrophobicity</t>
   </si>
   <si>
-    <t>hhHydrophobicityc</t>
+    <t>hhHydrophobicity</t>
   </si>
   <si>
-    <t>mfHydrophobicityd</t>
+    <t>mfHydrophobicity</t>
   </si>
   <si>
-    <t>ttHydrophobicitye</t>
+    <t>ttHydrophobicity</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>https://www.cgl.ucsf.edu/chimera/docs/UsersGuide/midas/hydrophob.html</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>From source</t>
+  </si>
+  <si>
+    <t>Mean(D, N)</t>
+  </si>
+  <si>
+    <t>Mean(E, Q)</t>
+  </si>
+  <si>
+    <t>Mean(All)</t>
+  </si>
+  <si>
+    <t>Set to 0</t>
   </si>
 </sst>
 </file>
@@ -185,12 +211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -508,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37354B2-B9FB-FA45-8F81-800BA5EE6A24}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7472,7 +7499,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9982,11 +10009,2525 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2B67AE-E669-F14D-8707-680391081833}">
+  <dimension ref="A1:Y25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <f>IF($A2=B$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.17</v>
+      </c>
+      <c r="C2" s="5">
+        <f>IF($A2=C$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.64</v>
+      </c>
+      <c r="D2" s="5">
+        <f>IF($A2=D$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.24999999999999997</v>
+      </c>
+      <c r="E2" s="5">
+        <f>IF($A2=E$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.06</v>
+      </c>
+      <c r="F2" s="5">
+        <f>IF($A2=F$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.41000000000000003</v>
+      </c>
+      <c r="G2" s="5">
+        <f>IF($A2=G$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.40999999999999992</v>
+      </c>
+      <c r="H2" s="5">
+        <f>IF($A2=H$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.85</v>
+      </c>
+      <c r="I2" s="5">
+        <f>IF($A2=I$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.16</v>
+      </c>
+      <c r="J2" s="5">
+        <f>IF($A2=J$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.78999999999999992</v>
+      </c>
+      <c r="K2" s="5">
+        <f>IF($A2=K$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.48</v>
+      </c>
+      <c r="L2" s="5">
+        <f>IF($A2=L$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.73000000000000009</v>
+      </c>
+      <c r="M2" s="5">
+        <f>IF($A2=M$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.82</v>
+      </c>
+      <c r="N2" s="5">
+        <f>IF($A2=N$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.4</v>
+      </c>
+      <c r="O2" s="5">
+        <f>IF($A2=O$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.2999999999999998</v>
+      </c>
+      <c r="P2" s="5">
+        <f>IF($A2=P$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>IF($A2=Q$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-4.0000000000000008E-2</v>
+      </c>
+      <c r="R2" s="5">
+        <f>IF($A2=R$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.03</v>
+      </c>
+      <c r="S2" s="5">
+        <f>IF($A2=S$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.02</v>
+      </c>
+      <c r="T2" s="5">
+        <f>IF($A2=T$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1099999999999999</v>
+      </c>
+      <c r="U2" s="5">
+        <f>IF($A2=U$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.1</v>
+      </c>
+      <c r="V2" s="5">
+        <f>IF($A2=V$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.65499999999999992</v>
+      </c>
+      <c r="W2" s="5">
+        <f>IF($A2=W$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="X2" s="5">
+        <f>IF($A2=X$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>5.0227272727272704E-2</v>
+      </c>
+      <c r="Y2" s="5">
+        <f>IF($A2=Y$1,VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A2,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <f>IF($A3=B$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.64</v>
+      </c>
+      <c r="C3" s="5">
+        <f>IF($A3=C$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.81</v>
+      </c>
+      <c r="D3" s="5">
+        <f>IF($A3=D$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.39000000000000007</v>
+      </c>
+      <c r="E3" s="5">
+        <f>IF($A3=E$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.41999999999999993</v>
+      </c>
+      <c r="F3" s="5">
+        <f>IF($A3=F$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.05</v>
+      </c>
+      <c r="G3" s="5">
+        <f>IF($A3=G$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.23000000000000009</v>
+      </c>
+      <c r="H3" s="5">
+        <f>IF($A3=H$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.21</v>
+      </c>
+      <c r="I3" s="5">
+        <f>IF($A3=I$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.8</v>
+      </c>
+      <c r="J3" s="5">
+        <f>IF($A3=J$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="K3" s="5">
+        <f>IF($A3=K$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1200000000000001</v>
+      </c>
+      <c r="L3" s="5">
+        <f>IF($A3=L$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.37</v>
+      </c>
+      <c r="M3" s="5">
+        <f>IF($A3=M$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.17999999999999994</v>
+      </c>
+      <c r="N3" s="5">
+        <f>IF($A3=N$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.04</v>
+      </c>
+      <c r="O3" s="5">
+        <f>IF($A3=O$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.94</v>
+      </c>
+      <c r="P3" s="5">
+        <f>IF($A3=P$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.36000000000000004</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>IF($A3=Q$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.68</v>
+      </c>
+      <c r="R3" s="5">
+        <f>IF($A3=R$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.67</v>
+      </c>
+      <c r="S3" s="5">
+        <f>IF($A3=S$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.66</v>
+      </c>
+      <c r="T3" s="5">
+        <f>IF($A3=T$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.75</v>
+      </c>
+      <c r="U3" s="5">
+        <f>IF($A3=U$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.74</v>
+      </c>
+      <c r="V3" s="5">
+        <f>IF($A3=V$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.4999999999999902E-2</v>
+      </c>
+      <c r="W3" s="5">
+        <f>IF($A3=W$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.49</v>
+      </c>
+      <c r="X3" s="5">
+        <f>IF($A3=X$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.58977272727272734</v>
+      </c>
+      <c r="Y3" s="5">
+        <f>IF($A3=Y$1,VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A3,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <f>IF($A4=B$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.24999999999999997</v>
+      </c>
+      <c r="C4" s="5">
+        <f>IF($A4=C$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.39000000000000007</v>
+      </c>
+      <c r="D4" s="5">
+        <f>IF($A4=D$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.42</v>
+      </c>
+      <c r="E4" s="5">
+        <f>IF($A4=E$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.81</v>
+      </c>
+      <c r="F4" s="5">
+        <f>IF($A4=F$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.65999999999999992</v>
+      </c>
+      <c r="G4" s="5">
+        <f>IF($A4=G$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.15999999999999998</v>
+      </c>
+      <c r="H4" s="5">
+        <f>IF($A4=H$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.6</v>
+      </c>
+      <c r="I4" s="5">
+        <f>IF($A4=I$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.41</v>
+      </c>
+      <c r="J4" s="5">
+        <f>IF($A4=J$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.54</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF($A4=K$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.73</v>
+      </c>
+      <c r="L4" s="5">
+        <f>IF($A4=L$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.98</v>
+      </c>
+      <c r="M4" s="5">
+        <f>IF($A4=M$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="N4" s="5">
+        <f>IF($A4=N$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.65</v>
+      </c>
+      <c r="O4" s="5">
+        <f>IF($A4=O$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.5499999999999998</v>
+      </c>
+      <c r="P4" s="5">
+        <f>IF($A4=P$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>IF($A4=Q$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="R4" s="5">
+        <f>IF($A4=R$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.27999999999999997</v>
+      </c>
+      <c r="S4" s="5">
+        <f>IF($A4=S$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.27</v>
+      </c>
+      <c r="T4" s="5">
+        <f>IF($A4=T$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.3599999999999999</v>
+      </c>
+      <c r="U4" s="5">
+        <f>IF($A4=U$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.35</v>
+      </c>
+      <c r="V4" s="5">
+        <f>IF($A4=V$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.40499999999999997</v>
+      </c>
+      <c r="W4" s="5">
+        <f>IF($A4=W$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="X4" s="5">
+        <f>IF($A4=X$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.19977272727272727</v>
+      </c>
+      <c r="Y4" s="5">
+        <f>IF($A4=Y$1,VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A4,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <f>IF($A5=B$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.06</v>
+      </c>
+      <c r="C5" s="5">
+        <f>IF($A5=C$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.41999999999999993</v>
+      </c>
+      <c r="D5" s="5">
+        <f>IF($A5=D$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.81</v>
+      </c>
+      <c r="E5" s="5">
+        <f>IF($A5=E$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.23</v>
+      </c>
+      <c r="F5" s="5">
+        <f>IF($A5=F$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.47</v>
+      </c>
+      <c r="G5" s="5">
+        <f>IF($A5=G$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.65</v>
+      </c>
+      <c r="H5" s="5">
+        <f>IF($A5=H$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.79</v>
+      </c>
+      <c r="I5" s="5">
+        <f>IF($A5=I$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.22</v>
+      </c>
+      <c r="J5" s="5">
+        <f>IF($A5=J$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.27</v>
+      </c>
+      <c r="K5" s="5">
+        <f>IF($A5=K$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.54</v>
+      </c>
+      <c r="L5" s="5">
+        <f>IF($A5=L$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.79</v>
+      </c>
+      <c r="M5" s="5">
+        <f>IF($A5=M$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.24</v>
+      </c>
+      <c r="N5" s="5">
+        <f>IF($A5=N$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.46</v>
+      </c>
+      <c r="O5" s="5">
+        <f>IF($A5=O$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.36</v>
+      </c>
+      <c r="P5" s="5">
+        <f>IF($A5=P$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.78</v>
+      </c>
+      <c r="Q5" s="5">
+        <f>IF($A5=Q$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="R5" s="5">
+        <f>IF($A5=R$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.0899999999999999</v>
+      </c>
+      <c r="S5" s="5">
+        <f>IF($A5=S$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-3.08</v>
+      </c>
+      <c r="T5" s="5">
+        <f>IF($A5=T$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.17</v>
+      </c>
+      <c r="U5" s="5">
+        <f>IF($A5=U$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="V5" s="5">
+        <f>IF($A5=V$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.40500000000000003</v>
+      </c>
+      <c r="W5" s="5">
+        <f>IF($A5=W$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>7.0000000000000062E-2</v>
+      </c>
+      <c r="X5" s="5">
+        <f>IF($A5=X$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.0097727272727273</v>
+      </c>
+      <c r="Y5" s="5">
+        <f>IF($A5=Y$1,VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A5,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <f>IF($A6=B$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="C6" s="5">
+        <f>IF($A6=C$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.05</v>
+      </c>
+      <c r="D6" s="5">
+        <f>IF($A6=D$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="E6" s="5">
+        <f>IF($A6=E$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.47</v>
+      </c>
+      <c r="F6" s="5">
+        <f>IF($A6=F$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.24</v>
+      </c>
+      <c r="G6" s="5">
+        <f>IF($A6=G$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.82</v>
+      </c>
+      <c r="H6" s="5">
+        <f>IF($A6=H$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I6" s="5">
+        <f>IF($A6=I$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.25</v>
+      </c>
+      <c r="J6" s="5">
+        <f>IF($A6=J$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.2</v>
+      </c>
+      <c r="K6" s="5">
+        <f>IF($A6=K$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="L6" s="5">
+        <f>IF($A6=L$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.32000000000000006</v>
+      </c>
+      <c r="M6" s="5">
+        <f>IF($A6=M$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.23</v>
+      </c>
+      <c r="N6" s="5">
+        <f>IF($A6=N$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>9.9999999999999811E-3</v>
+      </c>
+      <c r="O6" s="5">
+        <f>IF($A6=O$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.8899999999999999</v>
+      </c>
+      <c r="P6" s="5">
+        <f>IF($A6=P$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.69</v>
+      </c>
+      <c r="Q6" s="5">
+        <f>IF($A6=Q$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.37</v>
+      </c>
+      <c r="R6" s="5">
+        <f>IF($A6=R$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.38</v>
+      </c>
+      <c r="S6" s="5">
+        <f>IF($A6=S$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.61</v>
+      </c>
+      <c r="T6" s="5">
+        <f>IF($A6=T$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.7</v>
+      </c>
+      <c r="U6" s="5">
+        <f>IF($A6=U$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.31</v>
+      </c>
+      <c r="V6" s="5">
+        <f>IF($A6=V$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="W6" s="5">
+        <f>IF($A6=W$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.54</v>
+      </c>
+      <c r="X6" s="5">
+        <f>IF($A6=X$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.46022727272727271</v>
+      </c>
+      <c r="Y6" s="5">
+        <f>IF($A6=Y$1,VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A6,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <f>IF($A7=B$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.40999999999999992</v>
+      </c>
+      <c r="C7" s="5">
+        <f>IF($A7=C$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.23000000000000009</v>
+      </c>
+      <c r="D7" s="5">
+        <f>IF($A7=D$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.15999999999999998</v>
+      </c>
+      <c r="E7" s="5">
+        <f>IF($A7=E$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.65</v>
+      </c>
+      <c r="F7" s="5">
+        <f>IF($A7=F$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.82</v>
+      </c>
+      <c r="G7" s="5">
+        <f>IF($A7=G$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="H7" s="5">
+        <f>IF($A7=H$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.44</v>
+      </c>
+      <c r="I7" s="5">
+        <f>IF($A7=I$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="J7" s="5">
+        <f>IF($A7=J$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.38</v>
+      </c>
+      <c r="K7" s="5">
+        <f>IF($A7=K$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.8899999999999999</v>
+      </c>
+      <c r="L7" s="5">
+        <f>IF($A7=L$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1400000000000001</v>
+      </c>
+      <c r="M7" s="5">
+        <f>IF($A7=M$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="N7" s="5">
+        <f>IF($A7=N$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.80999999999999994</v>
+      </c>
+      <c r="O7" s="5">
+        <f>IF($A7=O$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.71</v>
+      </c>
+      <c r="P7" s="5">
+        <f>IF($A7=P$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.12999999999999995</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>IF($A7=Q$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.44999999999999996</v>
+      </c>
+      <c r="R7" s="5">
+        <f>IF($A7=R$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.43999999999999995</v>
+      </c>
+      <c r="S7" s="5">
+        <f>IF($A7=S$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.4300000000000002</v>
+      </c>
+      <c r="T7" s="5">
+        <f>IF($A7=T$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.52</v>
+      </c>
+      <c r="U7" s="5">
+        <f>IF($A7=U$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.51</v>
+      </c>
+      <c r="V7" s="5">
+        <f>IF($A7=V$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.245</v>
+      </c>
+      <c r="W7" s="5">
+        <f>IF($A7=W$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.72000000000000008</v>
+      </c>
+      <c r="X7" s="5">
+        <f>IF($A7=X$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.35977272727272724</v>
+      </c>
+      <c r="Y7" s="5">
+        <f>IF($A7=Y$1,VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A7,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.8899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <f>IF($A8=B$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.85</v>
+      </c>
+      <c r="C8" s="5">
+        <f>IF($A8=C$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.21</v>
+      </c>
+      <c r="D8" s="5">
+        <f>IF($A8=D$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.6</v>
+      </c>
+      <c r="E8" s="5">
+        <f>IF($A8=E$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.79</v>
+      </c>
+      <c r="F8" s="5">
+        <f>IF($A8=F$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.2599999999999998</v>
+      </c>
+      <c r="G8" s="5">
+        <f>IF($A8=G$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.44</v>
+      </c>
+      <c r="H8" s="5">
+        <f>IF($A8=H$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.02</v>
+      </c>
+      <c r="I8" s="5">
+        <f>IF($A8=I$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.0100000000000002</v>
+      </c>
+      <c r="J8" s="5">
+        <f>IF($A8=J$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.06</v>
+      </c>
+      <c r="K8" s="5">
+        <f>IF($A8=K$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.33</v>
+      </c>
+      <c r="L8" s="5">
+        <f>IF($A8=L$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.58</v>
+      </c>
+      <c r="M8" s="5">
+        <f>IF($A8=M$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.03</v>
+      </c>
+      <c r="N8" s="5">
+        <f>IF($A8=N$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.25</v>
+      </c>
+      <c r="O8" s="5">
+        <f>IF($A8=O$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-3.15</v>
+      </c>
+      <c r="P8" s="5">
+        <f>IF($A8=P$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.57</v>
+      </c>
+      <c r="Q8" s="5">
+        <f>IF($A8=Q$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.8900000000000001</v>
+      </c>
+      <c r="R8" s="5">
+        <f>IF($A8=R$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.88</v>
+      </c>
+      <c r="S8" s="5">
+        <f>IF($A8=S$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-3.87</v>
+      </c>
+      <c r="T8" s="5">
+        <f>IF($A8=T$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.96</v>
+      </c>
+      <c r="U8" s="5">
+        <f>IF($A8=U$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.95</v>
+      </c>
+      <c r="V8" s="5">
+        <f>IF($A8=V$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1950000000000001</v>
+      </c>
+      <c r="W8" s="5">
+        <f>IF($A8=W$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.72</v>
+      </c>
+      <c r="X8" s="5">
+        <f>IF($A8=X$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.7997727272727273</v>
+      </c>
+      <c r="Y8" s="5">
+        <f>IF($A8=Y$1,VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A8,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <f>IF($A9=B$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.16</v>
+      </c>
+      <c r="C9" s="5">
+        <f>IF($A9=C$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.8</v>
+      </c>
+      <c r="D9" s="5">
+        <f>IF($A9=D$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.41</v>
+      </c>
+      <c r="E9" s="5">
+        <f>IF($A9=E$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.22</v>
+      </c>
+      <c r="F9" s="5">
+        <f>IF($A9=F$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.25</v>
+      </c>
+      <c r="G9" s="5">
+        <f>IF($A9=G$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H9" s="5">
+        <f>IF($A9=H$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.0100000000000002</v>
+      </c>
+      <c r="I9" s="5">
+        <f>IF($A9=I$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.01</v>
+      </c>
+      <c r="J9" s="5">
+        <f>IF($A9=J$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.95</v>
+      </c>
+      <c r="K9" s="5">
+        <f>IF($A9=K$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.32</v>
+      </c>
+      <c r="L9" s="5">
+        <f>IF($A9=L$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.57000000000000006</v>
+      </c>
+      <c r="M9" s="5">
+        <f>IF($A9=M$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.98</v>
+      </c>
+      <c r="N9" s="5">
+        <f>IF($A9=N$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.24000000000000002</v>
+      </c>
+      <c r="O9" s="5">
+        <f>IF($A9=O$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="P9" s="5">
+        <f>IF($A9=P$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.44</v>
+      </c>
+      <c r="Q9" s="5">
+        <f>IF($A9=Q$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="R9" s="5">
+        <f>IF($A9=R$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.13</v>
+      </c>
+      <c r="S9" s="5">
+        <f>IF($A9=S$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.86</v>
+      </c>
+      <c r="T9" s="5">
+        <f>IF($A9=T$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.95</v>
+      </c>
+      <c r="U9" s="5">
+        <f>IF($A9=U$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="V9" s="5">
+        <f>IF($A9=V$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="W9" s="5">
+        <f>IF($A9=W$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.29</v>
+      </c>
+      <c r="X9" s="5">
+        <f>IF($A9=X$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.21022727272727271</v>
+      </c>
+      <c r="Y9" s="5">
+        <f>IF($A9=Y$1,VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A9,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <f>IF($A10=B$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.78999999999999992</v>
+      </c>
+      <c r="C10" s="5">
+        <f>IF($A10=C$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.14999999999999991</v>
+      </c>
+      <c r="D10" s="5">
+        <f>IF($A10=D$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.54</v>
+      </c>
+      <c r="E10" s="5">
+        <f>IF($A10=E$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.27</v>
+      </c>
+      <c r="F10" s="5">
+        <f>IF($A10=F$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.2</v>
+      </c>
+      <c r="G10" s="5">
+        <f>IF($A10=G$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.38</v>
+      </c>
+      <c r="H10" s="5">
+        <f>IF($A10=H$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.06</v>
+      </c>
+      <c r="I10" s="5">
+        <f>IF($A10=I$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.95</v>
+      </c>
+      <c r="J10" s="5">
+        <f>IF($A10=J$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.96</v>
+      </c>
+      <c r="K10" s="5">
+        <f>IF($A10=K$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.27</v>
+      </c>
+      <c r="L10" s="5">
+        <f>IF($A10=L$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.52</v>
+      </c>
+      <c r="M10" s="5">
+        <f>IF($A10=M$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="N10" s="5">
+        <f>IF($A10=N$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.19</v>
+      </c>
+      <c r="O10" s="5">
+        <f>IF($A10=O$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.09</v>
+      </c>
+      <c r="P10" s="5">
+        <f>IF($A10=P$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.51</v>
+      </c>
+      <c r="Q10" s="5">
+        <f>IF($A10=Q$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.83</v>
+      </c>
+      <c r="R10" s="5">
+        <f>IF($A10=R$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.82</v>
+      </c>
+      <c r="S10" s="5">
+        <f>IF($A10=S$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.81</v>
+      </c>
+      <c r="T10" s="5">
+        <f>IF($A10=T$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.9</v>
+      </c>
+      <c r="U10" s="5">
+        <f>IF($A10=U$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.8899999999999999</v>
+      </c>
+      <c r="V10" s="5">
+        <f>IF($A10=V$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="W10" s="5">
+        <f>IF($A10=W$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.34000000000000008</v>
+      </c>
+      <c r="X10" s="5">
+        <f>IF($A10=X$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.73977272727272725</v>
+      </c>
+      <c r="Y10" s="5">
+        <f>IF($A10=Y$1,VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A10,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <f>IF($A11=B$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.48</v>
+      </c>
+      <c r="C11" s="5">
+        <f>IF($A11=C$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D11" s="5">
+        <f>IF($A11=D$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.73</v>
+      </c>
+      <c r="E11" s="5">
+        <f>IF($A11=E$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.54</v>
+      </c>
+      <c r="F11" s="5">
+        <f>IF($A11=F$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <f>IF($A11=G$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="H11" s="5">
+        <f>IF($A11=H$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.33</v>
+      </c>
+      <c r="I11" s="5">
+        <f>IF($A11=I$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.32</v>
+      </c>
+      <c r="J11" s="5">
+        <f>IF($A11=J$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.27</v>
+      </c>
+      <c r="K11" s="5">
+        <f>IF($A11=K$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.31</v>
+      </c>
+      <c r="L11" s="5">
+        <f>IF($A11=L$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.25000000000000006</v>
+      </c>
+      <c r="M11" s="5">
+        <f>IF($A11=M$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.3</v>
+      </c>
+      <c r="N11" s="5">
+        <f>IF($A11=N$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>7.9999999999999988E-2</v>
+      </c>
+      <c r="O11" s="5">
+        <f>IF($A11=O$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.81999999999999984</v>
+      </c>
+      <c r="P11" s="5">
+        <f>IF($A11=P$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.76</v>
+      </c>
+      <c r="Q11" s="5">
+        <f>IF($A11=Q$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.44</v>
+      </c>
+      <c r="R11" s="5">
+        <f>IF($A11=R$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.45</v>
+      </c>
+      <c r="S11" s="5">
+        <f>IF($A11=S$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.54</v>
+      </c>
+      <c r="T11" s="5">
+        <f>IF($A11=T$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.62999999999999989</v>
+      </c>
+      <c r="U11" s="5">
+        <f>IF($A11=U$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.38</v>
+      </c>
+      <c r="V11" s="5">
+        <f>IF($A11=V$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.135</v>
+      </c>
+      <c r="W11" s="5">
+        <f>IF($A11=W$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.61</v>
+      </c>
+      <c r="X11" s="5">
+        <f>IF($A11=X$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.53022727272727277</v>
+      </c>
+      <c r="Y11" s="5">
+        <f>IF($A11=Y$1,VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A11,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <f>IF($A12=B$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.73000000000000009</v>
+      </c>
+      <c r="C12" s="5">
+        <f>IF($A12=C$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.37</v>
+      </c>
+      <c r="D12" s="5">
+        <f>IF($A12=D$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.98</v>
+      </c>
+      <c r="E12" s="5">
+        <f>IF($A12=E$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.79</v>
+      </c>
+      <c r="F12" s="5">
+        <f>IF($A12=F$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="G12" s="5">
+        <f>IF($A12=G$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="H12" s="5">
+        <f>IF($A12=H$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.58</v>
+      </c>
+      <c r="I12" s="5">
+        <f>IF($A12=I$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="J12" s="5">
+        <f>IF($A12=J$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.52</v>
+      </c>
+      <c r="K12" s="5">
+        <f>IF($A12=K$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="L12" s="5">
+        <f>IF($A12=L$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M12" s="5">
+        <f>IF($A12=M$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.55</v>
+      </c>
+      <c r="N12" s="5">
+        <f>IF($A12=N$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.33000000000000007</v>
+      </c>
+      <c r="O12" s="5">
+        <f>IF($A12=O$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.56999999999999984</v>
+      </c>
+      <c r="P12" s="5">
+        <f>IF($A12=P$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.01</v>
+      </c>
+      <c r="Q12" s="5">
+        <f>IF($A12=Q$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="R12" s="5">
+        <f>IF($A12=R$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="S12" s="5">
+        <f>IF($A12=S$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.29</v>
+      </c>
+      <c r="T12" s="5">
+        <f>IF($A12=T$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.37999999999999989</v>
+      </c>
+      <c r="U12" s="5">
+        <f>IF($A12=U$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.63000000000000012</v>
+      </c>
+      <c r="V12" s="5">
+        <f>IF($A12=V$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.385</v>
+      </c>
+      <c r="W12" s="5">
+        <f>IF($A12=W$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.86</v>
+      </c>
+      <c r="X12" s="5">
+        <f>IF($A12=X$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.78022727272727277</v>
+      </c>
+      <c r="Y12" s="5">
+        <f>IF($A12=Y$1,VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A12,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.25000000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <f>IF($A13=B$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.82</v>
+      </c>
+      <c r="C13" s="5">
+        <f>IF($A13=C$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.17999999999999994</v>
+      </c>
+      <c r="D13" s="5">
+        <f>IF($A13=D$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.57000000000000006</v>
+      </c>
+      <c r="E13" s="5">
+        <f>IF($A13=E$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.24</v>
+      </c>
+      <c r="F13" s="5">
+        <f>IF($A13=F$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.23</v>
+      </c>
+      <c r="G13" s="5">
+        <f>IF($A13=G$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.41000000000000003</v>
+      </c>
+      <c r="H13" s="5">
+        <f>IF($A13=H$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.03</v>
+      </c>
+      <c r="I13" s="5">
+        <f>IF($A13=I$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.98</v>
+      </c>
+      <c r="J13" s="5">
+        <f>IF($A13=J$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-3.0000000000000027E-2</v>
+      </c>
+      <c r="K13" s="5">
+        <f>IF($A13=K$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.3</v>
+      </c>
+      <c r="L13" s="5">
+        <f>IF($A13=L$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.55</v>
+      </c>
+      <c r="M13" s="5">
+        <f>IF($A13=M$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.99</v>
+      </c>
+      <c r="N13" s="5">
+        <f>IF($A13=N$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.22</v>
+      </c>
+      <c r="O13" s="5">
+        <f>IF($A13=O$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.12</v>
+      </c>
+      <c r="P13" s="5">
+        <f>IF($A13=P$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.54</v>
+      </c>
+      <c r="Q13" s="5">
+        <f>IF($A13=Q$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.86</v>
+      </c>
+      <c r="R13" s="5">
+        <f>IF($A13=R$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.85</v>
+      </c>
+      <c r="S13" s="5">
+        <f>IF($A13=S$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.84</v>
+      </c>
+      <c r="T13" s="5">
+        <f>IF($A13=T$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.93</v>
+      </c>
+      <c r="U13" s="5">
+        <f>IF($A13=U$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.91999999999999993</v>
+      </c>
+      <c r="V13" s="5">
+        <f>IF($A13=V$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.16500000000000004</v>
+      </c>
+      <c r="W13" s="5">
+        <f>IF($A13=W$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="X13" s="5">
+        <f>IF($A13=X$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.76977272727272728</v>
+      </c>
+      <c r="Y13" s="5">
+        <f>IF($A13=Y$1,VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A13,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5">
+        <f>IF($A14=B$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.4</v>
+      </c>
+      <c r="C14" s="5">
+        <f>IF($A14=C$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.04</v>
+      </c>
+      <c r="D14" s="5">
+        <f>IF($A14=D$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.65</v>
+      </c>
+      <c r="E14" s="5">
+        <f>IF($A14=E$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.46</v>
+      </c>
+      <c r="F14" s="5">
+        <f>IF($A14=F$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-9.9999999999999811E-3</v>
+      </c>
+      <c r="G14" s="5">
+        <f>IF($A14=G$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.80999999999999994</v>
+      </c>
+      <c r="H14" s="5">
+        <f>IF($A14=H$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.25</v>
+      </c>
+      <c r="I14" s="5">
+        <f>IF($A14=I$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="J14" s="5">
+        <f>IF($A14=J$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.19</v>
+      </c>
+      <c r="K14" s="5">
+        <f>IF($A14=K$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-7.9999999999999988E-2</v>
+      </c>
+      <c r="L14" s="5">
+        <f>IF($A14=L$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.33000000000000007</v>
+      </c>
+      <c r="M14" s="5">
+        <f>IF($A14=M$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.22</v>
+      </c>
+      <c r="N14" s="5">
+        <f>IF($A14=N$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.23</v>
+      </c>
+      <c r="O14" s="5">
+        <f>IF($A14=O$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="P14" s="5">
+        <f>IF($A14=P$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.68</v>
+      </c>
+      <c r="Q14" s="5">
+        <f>IF($A14=Q$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.36</v>
+      </c>
+      <c r="R14" s="5">
+        <f>IF($A14=R$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.37</v>
+      </c>
+      <c r="S14" s="5">
+        <f>IF($A14=S$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.62</v>
+      </c>
+      <c r="T14" s="5">
+        <f>IF($A14=T$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.71</v>
+      </c>
+      <c r="U14" s="5">
+        <f>IF($A14=U$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="V14" s="5">
+        <f>IF($A14=V$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="W14" s="5">
+        <f>IF($A14=W$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.53</v>
+      </c>
+      <c r="X14" s="5">
+        <f>IF($A14=X$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.4502272727272727</v>
+      </c>
+      <c r="Y14" s="5">
+        <f>IF($A14=Y$1,VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A14,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-7.9999999999999988E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5">
+        <f>IF($A15=B$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="C15" s="5">
+        <f>IF($A15=C$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.94</v>
+      </c>
+      <c r="D15" s="5">
+        <f>IF($A15=D$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.5499999999999998</v>
+      </c>
+      <c r="E15" s="5">
+        <f>IF($A15=E$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.36</v>
+      </c>
+      <c r="F15" s="5">
+        <f>IF($A15=F$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="G15" s="5">
+        <f>IF($A15=G$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.71</v>
+      </c>
+      <c r="H15" s="5">
+        <f>IF($A15=H$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>3.15</v>
+      </c>
+      <c r="I15" s="5">
+        <f>IF($A15=I$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="J15" s="5">
+        <f>IF($A15=J$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.09</v>
+      </c>
+      <c r="K15" s="5">
+        <f>IF($A15=K$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.81999999999999984</v>
+      </c>
+      <c r="L15" s="5">
+        <f>IF($A15=L$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.56999999999999984</v>
+      </c>
+      <c r="M15" s="5">
+        <f>IF($A15=M$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.12</v>
+      </c>
+      <c r="N15" s="5">
+        <f>IF($A15=N$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="O15" s="5">
+        <f>IF($A15=O$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="P15" s="5">
+        <f>IF($A15=P$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.5799999999999998</v>
+      </c>
+      <c r="Q15" s="5">
+        <f>IF($A15=Q$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.2599999999999998</v>
+      </c>
+      <c r="R15" s="5">
+        <f>IF($A15=R$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.27</v>
+      </c>
+      <c r="S15" s="5">
+        <f>IF($A15=S$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.7200000000000002</v>
+      </c>
+      <c r="T15" s="5">
+        <f>IF($A15=T$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.18999999999999995</v>
+      </c>
+      <c r="U15" s="5">
+        <f>IF($A15=U$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.2</v>
+      </c>
+      <c r="V15" s="5">
+        <f>IF($A15=V$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.9549999999999998</v>
+      </c>
+      <c r="W15" s="5">
+        <f>IF($A15=W$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.4299999999999997</v>
+      </c>
+      <c r="X15" s="5">
+        <f>IF($A15=X$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.3502272727272726</v>
+      </c>
+      <c r="Y15" s="5">
+        <f>IF($A15=Y$1,VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A15,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.81999999999999984</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5">
+        <f>IF($A16=B$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="C16" s="5">
+        <f>IF($A16=C$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.36000000000000004</v>
+      </c>
+      <c r="D16" s="5">
+        <f>IF($A16=D$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-3.0000000000000027E-2</v>
+      </c>
+      <c r="E16" s="5">
+        <f>IF($A16=E$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.78</v>
+      </c>
+      <c r="F16" s="5">
+        <f>IF($A16=F$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.69</v>
+      </c>
+      <c r="G16" s="5">
+        <f>IF($A16=G$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.12999999999999995</v>
+      </c>
+      <c r="H16" s="5">
+        <f>IF($A16=H$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.57</v>
+      </c>
+      <c r="I16" s="5">
+        <f>IF($A16=I$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.44</v>
+      </c>
+      <c r="J16" s="5">
+        <f>IF($A16=J$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.51</v>
+      </c>
+      <c r="K16" s="5">
+        <f>IF($A16=K$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.76</v>
+      </c>
+      <c r="L16" s="5">
+        <f>IF($A16=L$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.01</v>
+      </c>
+      <c r="M16" s="5">
+        <f>IF($A16=M$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.54</v>
+      </c>
+      <c r="N16" s="5">
+        <f>IF($A16=N$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.68</v>
+      </c>
+      <c r="O16" s="5">
+        <f>IF($A16=O$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.5799999999999998</v>
+      </c>
+      <c r="P16" s="5">
+        <f>IF($A16=P$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.45</v>
+      </c>
+      <c r="Q16" s="5">
+        <f>IF($A16=Q$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.32</v>
+      </c>
+      <c r="R16" s="5">
+        <f>IF($A16=R$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.31</v>
+      </c>
+      <c r="S16" s="5">
+        <f>IF($A16=S$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.3000000000000003</v>
+      </c>
+      <c r="T16" s="5">
+        <f>IF($A16=T$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.39</v>
+      </c>
+      <c r="U16" s="5">
+        <f>IF($A16=U$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.38</v>
+      </c>
+      <c r="V16" s="5">
+        <f>IF($A16=V$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.37499999999999994</v>
+      </c>
+      <c r="W16" s="5">
+        <f>IF($A16=W$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="X16" s="5">
+        <f>IF($A16=X$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.2297727272727273</v>
+      </c>
+      <c r="Y16" s="5">
+        <f>IF($A16=Y$1,VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A16,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <f>IF($A17=B$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="C17" s="5">
+        <f>IF($A17=C$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.68</v>
+      </c>
+      <c r="D17" s="5">
+        <f>IF($A17=D$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E17" s="5">
+        <f>IF($A17=E$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F17" s="5">
+        <f>IF($A17=F$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.37</v>
+      </c>
+      <c r="G17" s="5">
+        <f>IF($A17=G$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="H17" s="5">
+        <f>IF($A17=H$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="I17" s="5">
+        <f>IF($A17=I$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.12000000000000001</v>
+      </c>
+      <c r="J17" s="5">
+        <f>IF($A17=J$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.83</v>
+      </c>
+      <c r="K17" s="5">
+        <f>IF($A17=K$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.44</v>
+      </c>
+      <c r="L17" s="5">
+        <f>IF($A17=L$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.69000000000000006</v>
+      </c>
+      <c r="M17" s="5">
+        <f>IF($A17=M$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.86</v>
+      </c>
+      <c r="N17" s="5">
+        <f>IF($A17=N$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.36</v>
+      </c>
+      <c r="O17" s="5">
+        <f>IF($A17=O$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.2599999999999998</v>
+      </c>
+      <c r="P17" s="5">
+        <f>IF($A17=P$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.32</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>IF($A17=Q$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.13</v>
+      </c>
+      <c r="R17" s="5">
+        <f>IF($A17=R$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="S17" s="5">
+        <f>IF($A17=S$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.98</v>
+      </c>
+      <c r="T17" s="5">
+        <f>IF($A17=T$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.0699999999999998</v>
+      </c>
+      <c r="U17" s="5">
+        <f>IF($A17=U$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.06</v>
+      </c>
+      <c r="V17" s="5">
+        <f>IF($A17=V$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="W17" s="5">
+        <f>IF($A17=W$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.17</v>
+      </c>
+      <c r="X17" s="5">
+        <f>IF($A17=X$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>9.0227272727272712E-2</v>
+      </c>
+      <c r="Y17" s="5">
+        <f>IF($A17=Y$1,VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A17,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5">
+        <f>IF($A18=B$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.03</v>
+      </c>
+      <c r="C18" s="5">
+        <f>IF($A18=C$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.67</v>
+      </c>
+      <c r="D18" s="5">
+        <f>IF($A18=D$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="E18" s="5">
+        <f>IF($A18=E$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.0899999999999999</v>
+      </c>
+      <c r="F18" s="5">
+        <f>IF($A18=F$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.38</v>
+      </c>
+      <c r="G18" s="5">
+        <f>IF($A18=G$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.43999999999999995</v>
+      </c>
+      <c r="H18" s="5">
+        <f>IF($A18=H$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.88</v>
+      </c>
+      <c r="I18" s="5">
+        <f>IF($A18=I$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.13</v>
+      </c>
+      <c r="J18" s="5">
+        <f>IF($A18=J$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.82</v>
+      </c>
+      <c r="K18" s="5">
+        <f>IF($A18=K$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.45</v>
+      </c>
+      <c r="L18" s="5">
+        <f>IF($A18=L$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="M18" s="5">
+        <f>IF($A18=M$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.85</v>
+      </c>
+      <c r="N18" s="5">
+        <f>IF($A18=N$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.37</v>
+      </c>
+      <c r="O18" s="5">
+        <f>IF($A18=O$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.27</v>
+      </c>
+      <c r="P18" s="5">
+        <f>IF($A18=P$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.31</v>
+      </c>
+      <c r="Q18" s="5">
+        <f>IF($A18=Q$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="R18" s="5">
+        <f>IF($A18=R$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="S18" s="5">
+        <f>IF($A18=S$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.9900000000000002</v>
+      </c>
+      <c r="T18" s="5">
+        <f>IF($A18=T$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.08</v>
+      </c>
+      <c r="U18" s="5">
+        <f>IF($A18=U$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="V18" s="5">
+        <f>IF($A18=V$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.68499999999999994</v>
+      </c>
+      <c r="W18" s="5">
+        <f>IF($A18=W$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1600000000000001</v>
+      </c>
+      <c r="X18" s="5">
+        <f>IF($A18=X$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>8.0227272727272703E-2</v>
+      </c>
+      <c r="Y18" s="5">
+        <f>IF($A18=Y$1,VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A18,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5">
+        <f>IF($A19=B$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.02</v>
+      </c>
+      <c r="C19" s="5">
+        <f>IF($A19=C$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.66</v>
+      </c>
+      <c r="D19" s="5">
+        <f>IF($A19=D$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.27</v>
+      </c>
+      <c r="E19" s="5">
+        <f>IF($A19=E$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>3.08</v>
+      </c>
+      <c r="F19" s="5">
+        <f>IF($A19=F$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.61</v>
+      </c>
+      <c r="G19" s="5">
+        <f>IF($A19=G$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="H19" s="5">
+        <f>IF($A19=H$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>3.87</v>
+      </c>
+      <c r="I19" s="5">
+        <f>IF($A19=I$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.86</v>
+      </c>
+      <c r="J19" s="5">
+        <f>IF($A19=J$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.81</v>
+      </c>
+      <c r="K19" s="5">
+        <f>IF($A19=K$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.54</v>
+      </c>
+      <c r="L19" s="5">
+        <f>IF($A19=L$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.29</v>
+      </c>
+      <c r="M19" s="5">
+        <f>IF($A19=M$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.84</v>
+      </c>
+      <c r="N19" s="5">
+        <f>IF($A19=N$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.62</v>
+      </c>
+      <c r="O19" s="5">
+        <f>IF($A19=O$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.7200000000000002</v>
+      </c>
+      <c r="P19" s="5">
+        <f>IF($A19=P$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="Q19" s="5">
+        <f>IF($A19=Q$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.98</v>
+      </c>
+      <c r="R19" s="5">
+        <f>IF($A19=R$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.9900000000000002</v>
+      </c>
+      <c r="S19" s="5">
+        <f>IF($A19=S$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.85</v>
+      </c>
+      <c r="T19" s="5">
+        <f>IF($A19=T$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.91000000000000014</v>
+      </c>
+      <c r="U19" s="5">
+        <f>IF($A19=U$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.9200000000000002</v>
+      </c>
+      <c r="V19" s="5">
+        <f>IF($A19=V$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.6749999999999998</v>
+      </c>
+      <c r="W19" s="5">
+        <f>IF($A19=W$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="X19" s="5">
+        <f>IF($A19=X$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.0702272727272728</v>
+      </c>
+      <c r="Y19" s="5">
+        <f>IF($A19=Y$1,VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A19,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <f>IF($A20=B$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1099999999999999</v>
+      </c>
+      <c r="C20" s="5">
+        <f>IF($A20=C$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.75</v>
+      </c>
+      <c r="D20" s="5">
+        <f>IF($A20=D$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.3599999999999999</v>
+      </c>
+      <c r="E20" s="5">
+        <f>IF($A20=E$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.17</v>
+      </c>
+      <c r="F20" s="5">
+        <f>IF($A20=F$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.7</v>
+      </c>
+      <c r="G20" s="5">
+        <f>IF($A20=G$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.52</v>
+      </c>
+      <c r="H20" s="5">
+        <f>IF($A20=H$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.96</v>
+      </c>
+      <c r="I20" s="5">
+        <f>IF($A20=I$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.95</v>
+      </c>
+      <c r="J20" s="5">
+        <f>IF($A20=J$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.9</v>
+      </c>
+      <c r="K20" s="5">
+        <f>IF($A20=K$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="L20" s="5">
+        <f>IF($A20=L$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.37999999999999989</v>
+      </c>
+      <c r="M20" s="5">
+        <f>IF($A20=M$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.93</v>
+      </c>
+      <c r="N20" s="5">
+        <f>IF($A20=N$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.71</v>
+      </c>
+      <c r="O20" s="5">
+        <f>IF($A20=O$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.18999999999999995</v>
+      </c>
+      <c r="P20" s="5">
+        <f>IF($A20=P$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.39</v>
+      </c>
+      <c r="Q20" s="5">
+        <f>IF($A20=Q$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.0699999999999998</v>
+      </c>
+      <c r="R20" s="5">
+        <f>IF($A20=R$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.08</v>
+      </c>
+      <c r="S20" s="5">
+        <f>IF($A20=S$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.91000000000000014</v>
+      </c>
+      <c r="T20" s="5">
+        <f>IF($A20=T$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.94</v>
+      </c>
+      <c r="U20" s="5">
+        <f>IF($A20=U$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.01</v>
+      </c>
+      <c r="V20" s="5">
+        <f>IF($A20=V$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.7649999999999999</v>
+      </c>
+      <c r="W20" s="5">
+        <f>IF($A20=W$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="X20" s="5">
+        <f>IF($A20=X$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1602272727272727</v>
+      </c>
+      <c r="Y20" s="5">
+        <f>IF($A20=Y$1,VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A20,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.62999999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5">
+        <f>IF($A21=B$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="5">
+        <f>IF($A21=C$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.74</v>
+      </c>
+      <c r="D21" s="5">
+        <f>IF($A21=D$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.35</v>
+      </c>
+      <c r="E21" s="5">
+        <f>IF($A21=E$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F21" s="5">
+        <f>IF($A21=F$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.31</v>
+      </c>
+      <c r="G21" s="5">
+        <f>IF($A21=G$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.51</v>
+      </c>
+      <c r="H21" s="5">
+        <f>IF($A21=H$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.95</v>
+      </c>
+      <c r="I21" s="5">
+        <f>IF($A21=I$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-6.0000000000000005E-2</v>
+      </c>
+      <c r="J21" s="5">
+        <f>IF($A21=J$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="K21" s="5">
+        <f>IF($A21=K$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.38</v>
+      </c>
+      <c r="L21" s="5">
+        <f>IF($A21=L$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.63000000000000012</v>
+      </c>
+      <c r="M21" s="5">
+        <f>IF($A21=M$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="N21" s="5">
+        <f>IF($A21=N$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="O21" s="5">
+        <f>IF($A21=O$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.2</v>
+      </c>
+      <c r="P21" s="5">
+        <f>IF($A21=P$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.38</v>
+      </c>
+      <c r="Q21" s="5">
+        <f>IF($A21=Q$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.06</v>
+      </c>
+      <c r="R21" s="5">
+        <f>IF($A21=R$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S21" s="5">
+        <f>IF($A21=S$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.9200000000000002</v>
+      </c>
+      <c r="T21" s="5">
+        <f>IF($A21=T$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.01</v>
+      </c>
+      <c r="U21" s="5">
+        <f>IF($A21=U$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="V21" s="5">
+        <f>IF($A21=V$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.75499999999999989</v>
+      </c>
+      <c r="W21" s="5">
+        <f>IF($A21=W$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.23</v>
+      </c>
+      <c r="X21" s="5">
+        <f>IF($A21=X$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.15022727272727271</v>
+      </c>
+      <c r="Y21" s="5">
+        <f>IF($A21=Y$1,VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A21,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5">
+        <f>IF($A22=B$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.65499999999999992</v>
+      </c>
+      <c r="C22" s="5">
+        <f>IF($A22=C$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.4999999999999902E-2</v>
+      </c>
+      <c r="D22" s="5">
+        <f>IF($A22=D$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.40499999999999997</v>
+      </c>
+      <c r="E22" s="5">
+        <f>IF($A22=E$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="F22" s="5">
+        <f>IF($A22=F$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.0649999999999999</v>
+      </c>
+      <c r="G22" s="5">
+        <f>IF($A22=G$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.245</v>
+      </c>
+      <c r="H22" s="5">
+        <f>IF($A22=H$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1950000000000001</v>
+      </c>
+      <c r="I22" s="5">
+        <f>IF($A22=I$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.81499999999999995</v>
+      </c>
+      <c r="J22" s="5">
+        <f>IF($A22=J$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="K22" s="5">
+        <f>IF($A22=K$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.135</v>
+      </c>
+      <c r="L22" s="5">
+        <f>IF($A22=L$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.385</v>
+      </c>
+      <c r="M22" s="5">
+        <f>IF($A22=M$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.16500000000000004</v>
+      </c>
+      <c r="N22" s="5">
+        <f>IF($A22=N$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.0549999999999999</v>
+      </c>
+      <c r="O22" s="5">
+        <f>IF($A22=O$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.9549999999999998</v>
+      </c>
+      <c r="P22" s="5">
+        <f>IF($A22=P$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.37499999999999994</v>
+      </c>
+      <c r="Q22" s="5">
+        <f>IF($A22=Q$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.69499999999999995</v>
+      </c>
+      <c r="R22" s="5">
+        <f>IF($A22=R$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.68499999999999994</v>
+      </c>
+      <c r="S22" s="5">
+        <f>IF($A22=S$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.6749999999999998</v>
+      </c>
+      <c r="T22" s="5">
+        <f>IF($A22=T$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.7649999999999999</v>
+      </c>
+      <c r="U22" s="5">
+        <f>IF($A22=U$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.75499999999999989</v>
+      </c>
+      <c r="V22" s="5">
+        <f>IF($A22=V$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.82499999999999996</v>
+      </c>
+      <c r="W22" s="5">
+        <f>IF($A22=W$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.47500000000000009</v>
+      </c>
+      <c r="X22" s="5">
+        <f>IF($A22=X$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.60477272727272724</v>
+      </c>
+      <c r="Y22" s="5">
+        <f>IF($A22=Y$1,VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A22,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5">
+        <f>IF($A23=B$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1300000000000001</v>
+      </c>
+      <c r="C23" s="5">
+        <f>IF($A23=C$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.49</v>
+      </c>
+      <c r="D23" s="5">
+        <f>IF($A23=D$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.88000000000000012</v>
+      </c>
+      <c r="E23" s="5">
+        <f>IF($A23=E$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-7.0000000000000062E-2</v>
+      </c>
+      <c r="F23" s="5">
+        <f>IF($A23=F$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.54</v>
+      </c>
+      <c r="G23" s="5">
+        <f>IF($A23=G$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.72000000000000008</v>
+      </c>
+      <c r="H23" s="5">
+        <f>IF($A23=H$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.72</v>
+      </c>
+      <c r="I23" s="5">
+        <f>IF($A23=I$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.29</v>
+      </c>
+      <c r="J23" s="5">
+        <f>IF($A23=J$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.34000000000000008</v>
+      </c>
+      <c r="K23" s="5">
+        <f>IF($A23=K$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.61</v>
+      </c>
+      <c r="L23" s="5">
+        <f>IF($A23=L$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.86</v>
+      </c>
+      <c r="M23" s="5">
+        <f>IF($A23=M$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.31000000000000005</v>
+      </c>
+      <c r="N23" s="5">
+        <f>IF($A23=N$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.53</v>
+      </c>
+      <c r="O23" s="5">
+        <f>IF($A23=O$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.4299999999999997</v>
+      </c>
+      <c r="P23" s="5">
+        <f>IF($A23=P$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.85000000000000009</v>
+      </c>
+      <c r="Q23" s="5">
+        <f>IF($A23=Q$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.17</v>
+      </c>
+      <c r="R23" s="5">
+        <f>IF($A23=R$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1600000000000001</v>
+      </c>
+      <c r="S23" s="5">
+        <f>IF($A23=S$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-3.1500000000000004</v>
+      </c>
+      <c r="T23" s="5">
+        <f>IF($A23=T$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.2400000000000002</v>
+      </c>
+      <c r="U23" s="5">
+        <f>IF($A23=U$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.23</v>
+      </c>
+      <c r="V23" s="5">
+        <f>IF($A23=V$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.47500000000000009</v>
+      </c>
+      <c r="W23" s="5">
+        <f>IF($A23=W$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.3</v>
+      </c>
+      <c r="X23" s="5">
+        <f>IF($A23=X$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.0797727272727273</v>
+      </c>
+      <c r="Y23" s="5">
+        <f>IF($A23=Y$1,VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A23,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5">
+        <f>IF($A24=B$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-5.0227272727272704E-2</v>
+      </c>
+      <c r="C24" s="5">
+        <f>IF($A24=C$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.58977272727272734</v>
+      </c>
+      <c r="D24" s="5">
+        <f>IF($A24=D$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.19977272727272727</v>
+      </c>
+      <c r="E24" s="5">
+        <f>IF($A24=E$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.0097727272727273</v>
+      </c>
+      <c r="F24" s="5">
+        <f>IF($A24=F$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.46022727272727271</v>
+      </c>
+      <c r="G24" s="5">
+        <f>IF($A24=G$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.35977272727272724</v>
+      </c>
+      <c r="H24" s="5">
+        <f>IF($A24=H$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.7997727272727273</v>
+      </c>
+      <c r="I24" s="5">
+        <f>IF($A24=I$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.21022727272727271</v>
+      </c>
+      <c r="J24" s="5">
+        <f>IF($A24=J$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.73977272727272725</v>
+      </c>
+      <c r="K24" s="5">
+        <f>IF($A24=K$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.53022727272727277</v>
+      </c>
+      <c r="L24" s="5">
+        <f>IF($A24=L$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.78022727272727277</v>
+      </c>
+      <c r="M24" s="5">
+        <f>IF($A24=M$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.76977272727272728</v>
+      </c>
+      <c r="N24" s="5">
+        <f>IF($A24=N$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.4502272727272727</v>
+      </c>
+      <c r="O24" s="5">
+        <f>IF($A24=O$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.3502272727272726</v>
+      </c>
+      <c r="P24" s="5">
+        <f>IF($A24=P$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.2297727272727273</v>
+      </c>
+      <c r="Q24" s="5">
+        <f>IF($A24=Q$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-9.0227272727272712E-2</v>
+      </c>
+      <c r="R24" s="5">
+        <f>IF($A24=R$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-8.0227272727272703E-2</v>
+      </c>
+      <c r="S24" s="5">
+        <f>IF($A24=S$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-2.0702272727272728</v>
+      </c>
+      <c r="T24" s="5">
+        <f>IF($A24=T$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.1602272727272727</v>
+      </c>
+      <c r="U24" s="5">
+        <f>IF($A24=U$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.15022727272727271</v>
+      </c>
+      <c r="V24" s="5">
+        <f>IF($A24=V$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.60477272727272724</v>
+      </c>
+      <c r="W24" s="5">
+        <f>IF($A24=W$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.0797727272727273</v>
+      </c>
+      <c r="X24" s="5">
+        <f>IF($A24=X$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.22022727272727272</v>
+      </c>
+      <c r="Y24" s="5">
+        <f>IF($A24=Y$1,VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A24,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.53022727272727277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5">
+        <f>IF($A25=B$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(B$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.48</v>
+      </c>
+      <c r="C25" s="5">
+        <f>IF($A25=C$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(C$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D25" s="5">
+        <f>IF($A25=D$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(D$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.73</v>
+      </c>
+      <c r="E25" s="5">
+        <f>IF($A25=E$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(E$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.54</v>
+      </c>
+      <c r="F25" s="5">
+        <f>IF($A25=F$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(F$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G25" s="5">
+        <f>IF($A25=G$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(G$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="H25" s="5">
+        <f>IF($A25=H$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(H$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>2.33</v>
+      </c>
+      <c r="I25" s="5">
+        <f>IF($A25=I$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(I$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.32</v>
+      </c>
+      <c r="J25" s="5">
+        <f>IF($A25=J$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(J$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.27</v>
+      </c>
+      <c r="K25" s="5">
+        <f>IF($A25=K$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(K$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="5">
+        <f>IF($A25=L$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(L$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.25000000000000006</v>
+      </c>
+      <c r="M25" s="5">
+        <f>IF($A25=M$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(M$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.3</v>
+      </c>
+      <c r="N25" s="5">
+        <f>IF($A25=N$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(N$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>7.9999999999999988E-2</v>
+      </c>
+      <c r="O25" s="5">
+        <f>IF($A25=O$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(O$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.81999999999999984</v>
+      </c>
+      <c r="P25" s="5">
+        <f>IF($A25=P$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(P$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.76</v>
+      </c>
+      <c r="Q25" s="5">
+        <f>IF($A25=Q$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Q$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.44</v>
+      </c>
+      <c r="R25" s="5">
+        <f>IF($A25=R$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(R$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.45</v>
+      </c>
+      <c r="S25" s="5">
+        <f>IF($A25=S$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(S$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-1.54</v>
+      </c>
+      <c r="T25" s="5">
+        <f>IF($A25=T$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(T$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>-0.62999999999999989</v>
+      </c>
+      <c r="U25" s="5">
+        <f>IF($A25=U$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(U$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.38</v>
+      </c>
+      <c r="V25" s="5">
+        <f>IF($A25=V$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(V$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.135</v>
+      </c>
+      <c r="W25" s="5">
+        <f>IF($A25=W$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(W$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>1.61</v>
+      </c>
+      <c r="X25" s="5">
+        <f>IF($A25=X$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(X$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.53022727272727277</v>
+      </c>
+      <c r="Y25" s="5">
+        <f>IF($A25=Y$1,VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0),VLOOKUP($A25,'Hydrophobicity scales'!$A$2:$F$25,3,0)-VLOOKUP(Y$1,'Hydrophobicity scales'!$A$2:$F$25,3,0))</f>
+        <v>0.31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112F557F-3160-E940-BC16-A2D36F354CDD}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10000,7 +12541,7 @@
     <col min="7" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>24</v>
@@ -10017,8 +12558,11 @@
       <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -10037,8 +12581,11 @@
       <c r="F2" s="4">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -10057,8 +12604,11 @@
       <c r="F3" s="4">
         <v>1.46</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -10077,8 +12627,11 @@
       <c r="F4" s="4">
         <v>1.82</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -10097,8 +12650,11 @@
       <c r="F5" s="4">
         <v>1.98</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -10117,8 +12673,11 @@
       <c r="F6" s="4">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -10137,8 +12696,11 @@
       <c r="F7" s="4">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -10157,8 +12719,11 @@
       <c r="F8" s="4">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -10177,8 +12742,11 @@
       <c r="F9" s="4">
         <v>-0.19</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -10197,8 +12765,11 @@
       <c r="F10" s="4">
         <v>-0.32</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -10217,8 +12788,11 @@
       <c r="F11" s="4">
         <v>-0.53</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -10237,8 +12811,11 @@
       <c r="F12" s="4">
         <v>1.53</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -10257,8 +12834,11 @@
       <c r="F13" s="4">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -10277,8 +12857,11 @@
       <c r="F14" s="4">
         <v>-1.44</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -10297,8 +12880,11 @@
       <c r="F15" s="4">
         <v>-1.44</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -10317,8 +12903,11 @@
       <c r="F16" s="4">
         <v>-2.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -10337,8 +12926,11 @@
       <c r="F17" s="4">
         <v>-1.84</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -10357,8 +12949,11 @@
       <c r="F18" s="4">
         <v>-3.27</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -10377,8 +12972,11 @@
       <c r="F19" s="4">
         <v>-1.62</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -10397,8 +12995,11 @@
       <c r="F20" s="4">
         <v>-3.46</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
@@ -10416,6 +13017,124 @@
       </c>
       <c r="F21" s="4">
         <v>-2.57</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <f>SUM(B18,B19)/2</f>
+        <v>-3.5</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" ref="C22:F22" si="0">SUM(C18,C19)/2</f>
+        <v>-0.82499999999999996</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>2.77</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>3.21</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="0"/>
+        <v>-2.4450000000000003</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <f>SUM(B16,B17)/2</f>
+        <v>-3.5</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" ref="C23:F23" si="1">SUM(C16,C17)/2</f>
+        <v>-1.3</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="1"/>
+        <v>2.3249999999999997</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.37</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <f>SUM(B2:B23)/22</f>
+        <v>-0.76363636363636356</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" ref="C24:F24" si="2">SUM(C2:C23)/22</f>
+        <v>-0.22022727272727272</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="2"/>
+        <v>1.2104545454545457</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="2"/>
+        <v>1.1902272727272729</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.6211363636363636</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -10423,8 +13142,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2B67AE-E669-F14D-8707-680391081833}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549A4F79-BC58-1F4E-9FFB-47F04CA66FF8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EC315A-DC8C-5B4C-B4FC-08802FD6D664}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixed the irregular ise of tabs and spaces in encoding.py
</commit_message>
<xml_diff>
--- a/encoding_schemes.xlsx
+++ b/encoding_schemes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxc533/Documents/Arbejde/PhD/Kurser/Kursusmapper/Algorithms_in_Bioinformatics/Exercises/Algo/Algo2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC1CC26-0568-6141-85D7-2917C8F915F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817D9C46-2160-3445-9AB6-1070C147F5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="8" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOSUM50" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -265,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37354B2-B9FB-FA45-8F81-800BA5EE6A24}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3705,15 +3705,15 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <f>SUM(B17,B15)/2</f>
+        <f t="shared" ref="B22:D23" si="3">SUM(B17,B15)/2</f>
         <v>2.0549999999999997</v>
       </c>
       <c r="C22">
-        <f>SUM(C17,C15)/2</f>
+        <f t="shared" si="3"/>
         <v>9.31</v>
       </c>
       <c r="D22">
-        <f>SUM(D17,D15)/2</f>
+        <f t="shared" si="3"/>
         <v>1.93</v>
       </c>
       <c r="E22">
@@ -3733,15 +3733,15 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <f>SUM(B18,B16)/2</f>
+        <f t="shared" si="3"/>
         <v>2.1799999999999997</v>
       </c>
       <c r="C23">
-        <f>SUM(C18,C16)/2</f>
+        <f t="shared" si="3"/>
         <v>9.4</v>
       </c>
       <c r="D23">
-        <f>SUM(D18,D16)/2</f>
+        <f t="shared" si="3"/>
         <v>2.125</v>
       </c>
       <c r="E23">
@@ -21790,8 +21790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93462A1B-A6AF-8C4F-A55D-19C507D37BC5}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed encoding.py to handle different input structures, added single value encoding schemes in SINGLE, and moved other enocoding schemes to MULTIPLE
</commit_message>
<xml_diff>
--- a/encoding_schemes.xlsx
+++ b/encoding_schemes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxc533/Documents/Arbejde/PhD/Kurser/Kursusmapper/Algorithms_in_Bioinformatics/Exercises/Algo/Algo2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817D9C46-2160-3445-9AB6-1070C147F5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEA3CC3-7329-8B44-A104-912BED1EB011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" firstSheet="8" activeTab="13" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOSUM50" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,14 @@
     <sheet name="NTERM_CHARGE_PH7" sheetId="11" r:id="rId7"/>
     <sheet name="SIDECHAIN_CHARGE_PH7" sheetId="9" r:id="rId8"/>
     <sheet name="SIZE" sheetId="12" r:id="rId9"/>
-    <sheet name="Hydrophobicity scales" sheetId="5" r:id="rId10"/>
-    <sheet name="Charge" sheetId="7" r:id="rId11"/>
-    <sheet name="Size Lookup" sheetId="8" r:id="rId12"/>
+    <sheet name="SINGLE_SIZE" sheetId="14" r:id="rId10"/>
+    <sheet name="SINGLE_HYDROP_WWIHS" sheetId="13" r:id="rId11"/>
+    <sheet name="SINGLE_CTERM_CHARGE_PH7" sheetId="15" r:id="rId12"/>
+    <sheet name="SINGLE_NTERM_CHARGE_PH7" sheetId="16" r:id="rId13"/>
+    <sheet name="SINGLE_SIDECHAIN_CHARGE_PH7" sheetId="17" r:id="rId14"/>
+    <sheet name="Hydrophobicity scales" sheetId="5" r:id="rId15"/>
+    <sheet name="Charge" sheetId="7" r:id="rId16"/>
+    <sheet name="Size Lookup" sheetId="8" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="48">
   <si>
     <t>A</t>
   </si>
@@ -183,6 +188,12 @@
   </si>
   <si>
     <t>http://www.cbs.dtu.dk/services/NetPicoRNA/aa_table.php</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Mw(Da)</t>
   </si>
 </sst>
 </file>
@@ -586,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37354B2-B9FB-FA45-8F81-800BA5EE6A24}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2520,11 +2531,2887 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3319846C-F543-7041-A282-A04BEF802EBC}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="9">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="9">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f>SUM(B13,B4)/2</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B5,B15)/2</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f>SUM(B2:B23)/22</f>
+        <v>118.95454545454545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40625FE6-10A8-074C-BCD3-AB0BE419A670}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4">
+        <v>-0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4">
+        <v>-0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4">
+        <v>-0.96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>-2.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4">
+        <v>-0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="4">
+        <v>-1.23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4">
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="4">
+        <v>-0.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4">
+        <v>-0.81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>-0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>-0.22022727272727272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A1F7E3-1DD8-CF47-BCFC-017BF098CE9C}">
+  <dimension ref="A1:Y25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A2,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99997812286238008</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A3,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.9999852091348912</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A4,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998952882416614</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A5,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998769746364613</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A6,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99999487141246268</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A7,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.9999852091348912</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A8,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998451207369043</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A9,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99997812286238008</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A10,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99999339310917112</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A11,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99997709184826766</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A12,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99997709184826766</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A13,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998486461659886</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A14,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998094575589147</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A15,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99999323921595473</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A16,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99999022772328883</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A17,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998378216204897</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A18,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99995734386774304</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A19,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.999976012246236</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A20,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998415131926</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A21,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99997910747519814</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A22,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998865002066684</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A23,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99998486461659886</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A24,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.9999850769650771</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A25,Charge!$A$2:$G$25,5,0)</f>
+        <v>-0.99997812286238008</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62ECAF5-042F-764F-AF86-55F5D47D1C11}">
+  <dimension ref="A1:Y25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A2,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99796242225512743</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A3,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99096231626176035</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A4,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.98439833775817043</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A5,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99848872615708817</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A6,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99983406884697312</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A7,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99264144729182802</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A8,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99786659904087005</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A9,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99749440733271422</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A10,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99328457211076404</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A11,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99791505992637486</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A12,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99791505992637486</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A13,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.98890431113369226</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A14,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99387183593471762</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A15,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99264144729182802</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A16,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99974887443673854</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A17,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99297030856036073</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A18,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.9996286027580622</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A19,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99594272575704113</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A20,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99229732065999299</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A21,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99760690770954508</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A22,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99512608321838558</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A23,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99603471438084779</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A24,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99696390191913387</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A25,Charge!$A$2:$G$25,6,0)</f>
+        <v>0.99749440733271422</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F987709-BDB3-8A4E-A82E-9969BEF1E5A5}">
+  <dimension ref="A1:Y25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A2,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A3,Charge!$A$2:$G$25,7,0)</f>
+        <v>0.99999668869974989</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A4,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A5,Charge!$A$2:$G$25,7,0)</f>
+        <v>-0.99927608846747096</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A6,Charge!$A$2:$G$25,7,0)</f>
+        <v>-4.4683509371797249E-2</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A7,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A8,Charge!$A$2:$G$25,7,0)</f>
+        <v>-0.99822487725419018</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A9,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A10,Charge!$A$2:$G$25,7,0)</f>
+        <v>9.0909090909090939E-2</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A11,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A12,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A13,Charge!$A$2:$G$25,7,0)</f>
+        <v>0.99970496614799598</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A14,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A15,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A16,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A17,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A18,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A19,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A20,Charge!$A$2:$G$25,7,0)</f>
+        <v>-8.5041421831294072E-4</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A21,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A22,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A23,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A24,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6">
+        <f>VLOOKUP(SINGLE_CTERM_CHARGE_PH7!A25,Charge!$A$2:$G$25,7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112F557F-3160-E940-BC16-A2D36F354CDD}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C1" activeCellId="1" sqref="A1:A25 C1:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3139,12 +6026,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549A4F79-BC58-1F4E-9FFB-47F04CA66FF8}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E2" sqref="E2:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3820,12 +6707,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EC315A-DC8C-5B4C-B4FC-08802FD6D664}">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection sqref="A1:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11717,7 +14604,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y25"/>
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21791,7 +24678,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Actually added encode_parser to encode.py
</commit_message>
<xml_diff>
--- a/encoding_schemes.xlsx
+++ b/encoding_schemes.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxc533/Documents/Arbejde/PhD/Kurser/Kursusmapper/Algorithms_in_Bioinformatics/Exercises/Algo/Algo2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEA3CC3-7329-8B44-A104-912BED1EB011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB1874-F8AC-614B-86F3-1B4A973556BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" firstSheet="8" activeTab="13" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" firstSheet="2" activeTab="4" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOSUM50" sheetId="1" r:id="rId1"/>
     <sheet name="ONE_HOT" sheetId="2" r:id="rId2"/>
     <sheet name="ONE_HOT_MOD" sheetId="3" r:id="rId3"/>
     <sheet name="ONE_HOT_FRAC" sheetId="4" r:id="rId4"/>
-    <sheet name="HYDROP_WWIHS" sheetId="6" r:id="rId5"/>
+    <sheet name="HYDROPHOB" sheetId="6" r:id="rId5"/>
     <sheet name="CTERM_CHARGE_PH7" sheetId="10" r:id="rId6"/>
     <sheet name="NTERM_CHARGE_PH7" sheetId="11" r:id="rId7"/>
     <sheet name="SIDECHAIN_CHARGE_PH7" sheetId="9" r:id="rId8"/>
     <sheet name="SIZE" sheetId="12" r:id="rId9"/>
     <sheet name="SINGLE_SIZE" sheetId="14" r:id="rId10"/>
-    <sheet name="SINGLE_HYDROP_WWIHS" sheetId="13" r:id="rId11"/>
+    <sheet name="SINGLE_HYDROPHOB" sheetId="13" r:id="rId11"/>
     <sheet name="SINGLE_CTERM_CHARGE_PH7" sheetId="15" r:id="rId12"/>
     <sheet name="SINGLE_NTERM_CHARGE_PH7" sheetId="16" r:id="rId13"/>
     <sheet name="SINGLE_SIDECHAIN_CHARGE_PH7" sheetId="17" r:id="rId14"/>
@@ -2751,7 +2751,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B25"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4593,7 +4593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F987709-BDB3-8A4E-A82E-9969BEF1E5A5}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
@@ -14603,7 +14603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2B67AE-E669-F14D-8707-680391081833}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed SINGLE/SIZE to be scaled by mean and sd of all AA sizes
</commit_message>
<xml_diff>
--- a/encoding_schemes.xlsx
+++ b/encoding_schemes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxc533/Documents/Arbejde/PhD/Kurser/Kursusmapper/Algorithms_in_Bioinformatics/Exercises/Algo/Algo2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB1874-F8AC-614B-86F3-1B4A973556BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E350824-ECC3-6040-91E6-F814C5358E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" firstSheet="2" activeTab="4" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" firstSheet="8" activeTab="8" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOSUM50" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="49">
   <si>
     <t>A</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Mw(Da)</t>
+  </si>
+  <si>
+    <t>Scaled</t>
   </si>
 </sst>
 </file>
@@ -2535,7 +2538,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B25"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2551,7 +2554,8 @@
         <v>0</v>
       </c>
       <c r="B2" s="9">
-        <v>71</v>
+        <f>VLOOKUP(SINGLE_SIZE!A2,'Size Lookup'!A2:C25,3,0)</f>
+        <v>-1.6651214834421464</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2559,7 +2563,8 @@
         <v>4</v>
       </c>
       <c r="B3" s="9">
-        <v>103</v>
+        <f>VLOOKUP(SINGLE_SIZE!A3,'Size Lookup'!A3:C26,3,0)</f>
+        <v>-0.55398828501250552</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2567,7 +2572,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="9">
-        <v>114</v>
+        <f>VLOOKUP(SINGLE_SIZE!A4,'Size Lookup'!A4:C27,3,0)</f>
+        <v>-0.17203624805231651</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2575,7 +2581,8 @@
         <v>6</v>
       </c>
       <c r="B5" s="9">
-        <v>128</v>
+        <f>VLOOKUP(SINGLE_SIZE!A5,'Size Lookup'!A5:C28,3,0)</f>
+        <v>0.31408452626065136</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2583,7 +2590,8 @@
         <v>13</v>
       </c>
       <c r="B6" s="9">
-        <v>147</v>
+        <f>VLOOKUP(SINGLE_SIZE!A6,'Size Lookup'!A6:C29,3,0)</f>
+        <v>0.97381986282825062</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2591,7 +2599,8 @@
         <v>7</v>
       </c>
       <c r="B7" s="9">
-        <v>57</v>
+        <f>VLOOKUP(SINGLE_SIZE!A7,'Size Lookup'!A7:C30,3,0)</f>
+        <v>-2.151242257755114</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2599,7 +2608,8 @@
         <v>8</v>
       </c>
       <c r="B8" s="9">
-        <v>137</v>
+        <f>VLOOKUP(SINGLE_SIZE!A8,'Size Lookup'!A8:C31,3,0)</f>
+        <v>0.62659073831898782</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2607,7 +2617,8 @@
         <v>9</v>
       </c>
       <c r="B9" s="9">
-        <v>113</v>
+        <f>VLOOKUP(SINGLE_SIZE!A9,'Size Lookup'!A9:C32,3,0)</f>
+        <v>-0.20675916050324278</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2615,7 +2626,8 @@
         <v>11</v>
       </c>
       <c r="B10" s="9">
-        <v>129</v>
+        <f>VLOOKUP(SINGLE_SIZE!A10,'Size Lookup'!A10:C33,3,0)</f>
+        <v>0.34880743871157766</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2623,7 +2635,8 @@
         <v>10</v>
       </c>
       <c r="B11" s="9">
-        <v>113</v>
+        <f>VLOOKUP(SINGLE_SIZE!A11,'Size Lookup'!A11:C34,3,0)</f>
+        <v>-0.20675916050324278</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2631,7 +2644,8 @@
         <v>12</v>
       </c>
       <c r="B12" s="9">
-        <v>131</v>
+        <f>VLOOKUP(SINGLE_SIZE!A12,'Size Lookup'!A12:C35,3,0)</f>
+        <v>0.41825326361343018</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2639,7 +2653,8 @@
         <v>2</v>
       </c>
       <c r="B13" s="9">
-        <v>114</v>
+        <f>VLOOKUP(SINGLE_SIZE!A13,'Size Lookup'!A13:C36,3,0)</f>
+        <v>-0.17203624805231651</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2647,7 +2662,8 @@
         <v>14</v>
       </c>
       <c r="B14" s="9">
-        <v>97</v>
+        <f>VLOOKUP(SINGLE_SIZE!A14,'Size Lookup'!A14:C37,3,0)</f>
+        <v>-0.76232575971806316</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2655,7 +2671,8 @@
         <v>5</v>
       </c>
       <c r="B15" s="9">
-        <v>128</v>
+        <f>VLOOKUP(SINGLE_SIZE!A15,'Size Lookup'!A15:C38,3,0)</f>
+        <v>0.31408452626065136</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2663,7 +2680,8 @@
         <v>1</v>
       </c>
       <c r="B16" s="9">
-        <v>157</v>
+        <f>VLOOKUP(SINGLE_SIZE!A16,'Size Lookup'!A16:C39,3,0)</f>
+        <v>1.3210489873375133</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2671,7 +2689,8 @@
         <v>15</v>
       </c>
       <c r="B17" s="9">
-        <v>87</v>
+        <f>VLOOKUP(SINGLE_SIZE!A17,'Size Lookup'!A17:C40,3,0)</f>
+        <v>-1.109554884227326</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2679,7 +2698,8 @@
         <v>16</v>
       </c>
       <c r="B18" s="9">
-        <v>101</v>
+        <f>VLOOKUP(SINGLE_SIZE!A18,'Size Lookup'!A18:C41,3,0)</f>
+        <v>-0.6234341099143581</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2687,7 +2707,8 @@
         <v>19</v>
       </c>
       <c r="B19" s="9">
-        <v>99</v>
+        <f>VLOOKUP(SINGLE_SIZE!A19,'Size Lookup'!A19:C42,3,0)</f>
+        <v>-0.69287993481621069</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2695,7 +2716,8 @@
         <v>17</v>
       </c>
       <c r="B20" s="9">
-        <v>186</v>
+        <f>VLOOKUP(SINGLE_SIZE!A20,'Size Lookup'!A20:C43,3,0)</f>
+        <v>2.3280134484143753</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2703,34 +2725,35 @@
         <v>18</v>
       </c>
       <c r="B21" s="9">
-        <v>163</v>
+        <f>VLOOKUP(SINGLE_SIZE!A21,'Size Lookup'!A21:C44,3,0)</f>
+        <v>1.529386462043071</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <f>SUM(B13,B4)/2</f>
-        <v>114</v>
+      <c r="B22" s="9">
+        <f>VLOOKUP(SINGLE_SIZE!A22,'Size Lookup'!A22:C45,3,0)</f>
+        <v>-0.17203624805231651</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <f>SUM(B5,B15)/2</f>
-        <v>128</v>
+      <c r="B23" s="9">
+        <f>VLOOKUP(SINGLE_SIZE!A23,'Size Lookup'!A23:C46,3,0)</f>
+        <v>0.31408452626065136</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <f>SUM(B2:B23)/22</f>
-        <v>118.95454545454545</v>
+      <c r="B24" s="9">
+        <f>VLOOKUP(SINGLE_SIZE!A24,'Size Lookup'!A24:C47,3,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -6031,7 +6054,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E25"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6712,7 +6735,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B25"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6727,7 +6750,9 @@
       <c r="B1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -6741,7 +6766,10 @@
       <c r="B2" s="9">
         <v>71</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="7">
+        <f>(B2-SUM($B$2:$B$24)/COUNT($B$2:$B$24))/STDEV($B$2:$B$24)</f>
+        <v>-1.6651214834421464</v>
+      </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -6755,7 +6783,10 @@
       <c r="B3" s="9">
         <v>103</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C24" si="0">(B3-SUM($B$2:$B$24)/COUNT($B$2:$B$24))/STDEV($B$2:$B$24)</f>
+        <v>-0.55398828501250552</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -6769,7 +6800,10 @@
       <c r="B4" s="9">
         <v>114</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.17203624805231651</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -6783,7 +6817,10 @@
       <c r="B5" s="9">
         <v>128</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.31408452626065136</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -6797,7 +6834,10 @@
       <c r="B6" s="9">
         <v>147</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.97381986282825062</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -6811,7 +6851,10 @@
       <c r="B7" s="9">
         <v>57</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>-2.151242257755114</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -6825,7 +6868,10 @@
       <c r="B8" s="9">
         <v>137</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.62659073831898782</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -6839,7 +6885,10 @@
       <c r="B9" s="9">
         <v>113</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.20675916050324278</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -6853,7 +6902,10 @@
       <c r="B10" s="9">
         <v>129</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.34880743871157766</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -6867,7 +6919,10 @@
       <c r="B11" s="9">
         <v>113</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.20675916050324278</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -6881,7 +6936,10 @@
       <c r="B12" s="9">
         <v>131</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41825326361343018</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -6895,7 +6953,10 @@
       <c r="B13" s="9">
         <v>114</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.17203624805231651</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -6909,7 +6970,10 @@
       <c r="B14" s="9">
         <v>97</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.76232575971806316</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -6923,7 +6987,10 @@
       <c r="B15" s="9">
         <v>128</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.31408452626065136</v>
+      </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -6937,7 +7004,10 @@
       <c r="B16" s="9">
         <v>157</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3210489873375133</v>
+      </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -6951,7 +7021,10 @@
       <c r="B17" s="9">
         <v>87</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>-1.109554884227326</v>
+      </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -6965,7 +7038,10 @@
       <c r="B18" s="9">
         <v>101</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.6234341099143581</v>
+      </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -6979,7 +7055,10 @@
       <c r="B19" s="9">
         <v>99</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.69287993481621069</v>
+      </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -6993,7 +7072,10 @@
       <c r="B20" s="9">
         <v>186</v>
       </c>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7">
+        <f t="shared" si="0"/>
+        <v>2.3280134484143753</v>
+      </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -7007,7 +7089,10 @@
       <c r="B21" s="9">
         <v>163</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="7">
+        <f t="shared" si="0"/>
+        <v>1.529386462043071</v>
+      </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -7022,6 +7107,10 @@
         <f>SUM(B13,B4)/2</f>
         <v>114</v>
       </c>
+      <c r="C22" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.17203624805231651</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
@@ -7031,6 +7120,10 @@
         <f>SUM(B5,B15)/2</f>
         <v>128</v>
       </c>
+      <c r="C23" s="7">
+        <f t="shared" si="0"/>
+        <v>0.31408452626065136</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
@@ -7039,6 +7132,10 @@
       <c r="B24">
         <f>SUM(B2:B23)/22</f>
         <v>118.95454545454545</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -14603,7 +14700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2B67AE-E669-F14D-8707-680391081833}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
@@ -24677,8 +24774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93462A1B-A6AF-8C4F-A55D-19C507D37BC5}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24774,99 +24871,99 @@
         <v>0</v>
       </c>
       <c r="B2" s="5">
-        <f>IF($A2=B$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>71</v>
+        <f>IF($A2=B$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.6651214834421464</v>
       </c>
       <c r="C2" s="5">
-        <f>IF($A2=C$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>86</v>
+        <f>IF($A2=C$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.9861704707796597</v>
       </c>
       <c r="D2" s="5">
-        <f>IF($A2=D$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A2=D$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="E2" s="5">
-        <f>IF($A2=E$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A2=E$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="F2" s="5">
-        <f>IF($A2=F$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>32</v>
+        <f>IF($A2=F$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1111331984296409</v>
       </c>
       <c r="G2" s="5">
-        <f>IF($A2=G$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A2=G$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027977</v>
       </c>
       <c r="H2" s="5">
-        <f>IF($A2=H$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A2=H$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027977</v>
       </c>
       <c r="I2" s="5">
-        <f>IF($A2=I$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A2=I$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296763</v>
       </c>
       <c r="J2" s="5">
-        <f>IF($A2=J$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>66</v>
+        <f>IF($A2=J$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.2917122217611343</v>
       </c>
       <c r="K2" s="5">
-        <f>IF($A2=K$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>42</v>
+        <f>IF($A2=K$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4583623229389036</v>
       </c>
       <c r="L2" s="5">
-        <f>IF($A2=L$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>42</v>
+        <f>IF($A2=L$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4583623229389036</v>
       </c>
       <c r="M2" s="5">
-        <f>IF($A2=M$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>58</v>
+        <f>IF($A2=M$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.013928922153724</v>
       </c>
       <c r="N2" s="5">
-        <f>IF($A2=N$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>60</v>
+        <f>IF($A2=N$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.0833747470555766</v>
       </c>
       <c r="O2" s="5">
-        <f>IF($A2=O$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>76</v>
+        <f>IF($A2=O$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.6389413462703972</v>
       </c>
       <c r="P2" s="5">
-        <f>IF($A2=P$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>26</v>
+        <f>IF($A2=P$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.90279572372408323</v>
       </c>
       <c r="Q2" s="5">
-        <f>IF($A2=Q$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A2=Q$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="R2" s="5">
-        <f>IF($A2=R$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>30</v>
+        <f>IF($A2=R$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0416873735277883</v>
       </c>
       <c r="S2" s="5">
-        <f>IF($A2=S$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>115</v>
+        <f>IF($A2=S$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.9931349318565217</v>
       </c>
       <c r="T2" s="5">
-        <f>IF($A2=T$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>92</v>
+        <f>IF($A2=T$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.1945079454852174</v>
       </c>
       <c r="U2" s="5">
-        <f>IF($A2=U$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>28</v>
+        <f>IF($A2=U$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.9722415486259357</v>
       </c>
       <c r="V2" s="5">
-        <f>IF($A2=V$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A2=V$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="W2" s="5">
-        <f>IF($A2=W$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A2=W$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027977</v>
       </c>
       <c r="X2" s="5">
-        <f>IF($A2=X$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>47.954545454545453</v>
+        <f>IF($A2=X$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.6651214834421464</v>
       </c>
       <c r="Y2" s="5">
-        <f>IF($A2=Y$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A2=Y$1,VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A2,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -24875,100 +24972,100 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <f>IF($A3=B$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-86</v>
+        <f>IF($A3=B$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.9861704707796597</v>
       </c>
       <c r="C3" s="5">
-        <f>IF($A3=C$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>157</v>
+        <f>IF($A3=C$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.3210489873375133</v>
       </c>
       <c r="D3" s="5">
-        <f>IF($A3=D$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A3=D$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
       <c r="E3" s="5">
-        <f>IF($A3=E$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A3=E$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
       <c r="F3" s="5">
-        <f>IF($A3=F$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-54</v>
+        <f>IF($A3=F$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.8750372723500188</v>
       </c>
       <c r="G3" s="5">
-        <f>IF($A3=G$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-29</v>
+        <f>IF($A3=G$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.006964461076862</v>
       </c>
       <c r="H3" s="5">
-        <f>IF($A3=H$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-29</v>
+        <f>IF($A3=H$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.006964461076862</v>
       </c>
       <c r="I3" s="5">
-        <f>IF($A3=I$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-100</v>
+        <f>IF($A3=I$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926273</v>
       </c>
       <c r="J3" s="5">
-        <f>IF($A3=J$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-20</v>
+        <f>IF($A3=J$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.69445824901852549</v>
       </c>
       <c r="K3" s="5">
-        <f>IF($A3=K$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-44</v>
+        <f>IF($A3=K$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.5278081478407561</v>
       </c>
       <c r="L3" s="5">
-        <f>IF($A3=L$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-44</v>
+        <f>IF($A3=L$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.5278081478407561</v>
       </c>
       <c r="M3" s="5">
-        <f>IF($A3=M$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-28</v>
+        <f>IF($A3=M$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.9722415486259357</v>
       </c>
       <c r="N3" s="5">
-        <f>IF($A3=N$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-26</v>
+        <f>IF($A3=N$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.90279572372408312</v>
       </c>
       <c r="O3" s="5">
-        <f>IF($A3=O$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-10</v>
+        <f>IF($A3=O$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.34722912450926269</v>
       </c>
       <c r="P3" s="5">
-        <f>IF($A3=P$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-60</v>
+        <f>IF($A3=P$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.0833747470555766</v>
       </c>
       <c r="Q3" s="5">
-        <f>IF($A3=Q$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-70</v>
+        <f>IF($A3=Q$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.4306038715648395</v>
       </c>
       <c r="R3" s="5">
-        <f>IF($A3=R$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-56</v>
+        <f>IF($A3=R$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9444830972518714</v>
       </c>
       <c r="S3" s="5">
-        <f>IF($A3=S$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>29</v>
+        <f>IF($A3=S$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.006964461076862</v>
       </c>
       <c r="T3" s="5">
-        <f>IF($A3=T$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>6</v>
+        <f>IF($A3=T$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.20833747470555775</v>
       </c>
       <c r="U3" s="5">
-        <f>IF($A3=U$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-58</v>
+        <f>IF($A3=U$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.013928922153724</v>
       </c>
       <c r="V3" s="5">
-        <f>IF($A3=V$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A3=V$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
       <c r="W3" s="5">
-        <f>IF($A3=W$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-29</v>
+        <f>IF($A3=W$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.006964461076862</v>
       </c>
       <c r="X3" s="5">
-        <f>IF($A3=X$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-38.045454545454547</v>
+        <f>IF($A3=X$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.3210489873375133</v>
       </c>
       <c r="Y3" s="5">
-        <f>IF($A3=Y$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-86</v>
+        <f>IF($A3=Y$1,VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A3,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.9861704707796597</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -24976,100 +25073,100 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <f>IF($A4=B$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A4=B$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
       <c r="C4" s="5">
-        <f>IF($A4=C$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A4=C$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="D4" s="5">
-        <f>IF($A4=D$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>114</v>
+        <f>IF($A4=D$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.17203624805231651</v>
       </c>
       <c r="E4" s="5">
-        <f>IF($A4=E$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A4=E$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="F4" s="5">
-        <f>IF($A4=F$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-11</v>
+        <f>IF($A4=F$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.38195203696018898</v>
       </c>
       <c r="G4" s="5">
-        <f>IF($A4=G$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A4=G$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="H4" s="5">
-        <f>IF($A4=H$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A4=H$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="I4" s="5">
-        <f>IF($A4=I$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A4=I$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027975</v>
       </c>
       <c r="J4" s="5">
-        <f>IF($A4=J$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>23</v>
+        <f>IF($A4=J$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.79862698637130436</v>
       </c>
       <c r="K4" s="5">
-        <f>IF($A4=K$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A4=K$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926263E-2</v>
       </c>
       <c r="L4" s="5">
-        <f>IF($A4=L$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A4=L$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926263E-2</v>
       </c>
       <c r="M4" s="5">
-        <f>IF($A4=M$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A4=M$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="N4" s="5">
-        <f>IF($A4=N$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>17</v>
+        <f>IF($A4=N$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.59028951166574672</v>
       </c>
       <c r="O4" s="5">
-        <f>IF($A4=O$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>33</v>
+        <f>IF($A4=O$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1458561108805672</v>
       </c>
       <c r="P4" s="5">
-        <f>IF($A4=P$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-17</v>
+        <f>IF($A4=P$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.59028951166574661</v>
       </c>
       <c r="Q4" s="5">
-        <f>IF($A4=Q$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-27</v>
+        <f>IF($A4=Q$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.93751863617500941</v>
       </c>
       <c r="R4" s="5">
-        <f>IF($A4=R$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-13</v>
+        <f>IF($A4=R$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.45139786186204156</v>
       </c>
       <c r="S4" s="5">
-        <f>IF($A4=S$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>72</v>
+        <f>IF($A4=S$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.5000496964666916</v>
       </c>
       <c r="T4" s="5">
-        <f>IF($A4=T$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>49</v>
+        <f>IF($A4=T$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7014227100953876</v>
       </c>
       <c r="U4" s="5">
-        <f>IF($A4=U$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A4=U$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="V4" s="5">
-        <f>IF($A4=V$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A4=V$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="W4" s="5">
-        <f>IF($A4=W$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A4=W$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="X4" s="5">
-        <f>IF($A4=X$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>4.9545454545454533</v>
+        <f>IF($A4=X$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.17203624805231651</v>
       </c>
       <c r="Y4" s="5">
-        <f>IF($A4=Y$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A4=Y$1,VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A4,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
@@ -25077,100 +25174,100 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <f>IF($A5=B$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A5=B$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
       <c r="C5" s="5">
-        <f>IF($A5=C$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A5=C$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="D5" s="5">
-        <f>IF($A5=D$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A5=D$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="E5" s="5">
-        <f>IF($A5=E$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>114</v>
+        <f>IF($A5=E$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.17203624805231651</v>
       </c>
       <c r="F5" s="5">
-        <f>IF($A5=F$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-11</v>
+        <f>IF($A5=F$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.38195203696018898</v>
       </c>
       <c r="G5" s="5">
-        <f>IF($A5=G$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A5=G$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="H5" s="5">
-        <f>IF($A5=H$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A5=H$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="I5" s="5">
-        <f>IF($A5=I$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A5=I$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027975</v>
       </c>
       <c r="J5" s="5">
-        <f>IF($A5=J$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>23</v>
+        <f>IF($A5=J$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.79862698637130436</v>
       </c>
       <c r="K5" s="5">
-        <f>IF($A5=K$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A5=K$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926263E-2</v>
       </c>
       <c r="L5" s="5">
-        <f>IF($A5=L$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A5=L$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926263E-2</v>
       </c>
       <c r="M5" s="5">
-        <f>IF($A5=M$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A5=M$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="N5" s="5">
-        <f>IF($A5=N$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>17</v>
+        <f>IF($A5=N$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.59028951166574672</v>
       </c>
       <c r="O5" s="5">
-        <f>IF($A5=O$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>33</v>
+        <f>IF($A5=O$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1458561108805672</v>
       </c>
       <c r="P5" s="5">
-        <f>IF($A5=P$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-17</v>
+        <f>IF($A5=P$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.59028951166574661</v>
       </c>
       <c r="Q5" s="5">
-        <f>IF($A5=Q$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-27</v>
+        <f>IF($A5=Q$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.93751863617500941</v>
       </c>
       <c r="R5" s="5">
-        <f>IF($A5=R$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-13</v>
+        <f>IF($A5=R$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.45139786186204156</v>
       </c>
       <c r="S5" s="5">
-        <f>IF($A5=S$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>72</v>
+        <f>IF($A5=S$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.5000496964666916</v>
       </c>
       <c r="T5" s="5">
-        <f>IF($A5=T$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>49</v>
+        <f>IF($A5=T$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7014227100953876</v>
       </c>
       <c r="U5" s="5">
-        <f>IF($A5=U$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A5=U$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="V5" s="5">
-        <f>IF($A5=V$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A5=V$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="W5" s="5">
-        <f>IF($A5=W$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A5=W$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="X5" s="5">
-        <f>IF($A5=X$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>4.9545454545454533</v>
+        <f>IF($A5=X$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.17203624805231651</v>
       </c>
       <c r="Y5" s="5">
-        <f>IF($A5=Y$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A5=Y$1,VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A5,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
@@ -25178,100 +25275,100 @@
         <v>4</v>
       </c>
       <c r="B6" s="5">
-        <f>IF($A6=B$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-32</v>
+        <f>IF($A6=B$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1111331984296409</v>
       </c>
       <c r="C6" s="5">
-        <f>IF($A6=C$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>54</v>
+        <f>IF($A6=C$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.8750372723500188</v>
       </c>
       <c r="D6" s="5">
-        <f>IF($A6=D$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>11</v>
+        <f>IF($A6=D$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.38195203696018898</v>
       </c>
       <c r="E6" s="5">
-        <f>IF($A6=E$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>11</v>
+        <f>IF($A6=E$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.38195203696018898</v>
       </c>
       <c r="F6" s="5">
-        <f>IF($A6=F$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>103</v>
+        <f>IF($A6=F$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55398828501250552</v>
       </c>
       <c r="G6" s="5">
-        <f>IF($A6=G$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>25</v>
+        <f>IF($A6=G$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.86807281127315683</v>
       </c>
       <c r="H6" s="5">
-        <f>IF($A6=H$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>25</v>
+        <f>IF($A6=H$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.86807281127315683</v>
       </c>
       <c r="I6" s="5">
-        <f>IF($A6=I$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-46</v>
+        <f>IF($A6=I$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.5972539727426085</v>
       </c>
       <c r="J6" s="5">
-        <f>IF($A6=J$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>34</v>
+        <f>IF($A6=J$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1805790233314934</v>
       </c>
       <c r="K6" s="5">
-        <f>IF($A6=K$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>10</v>
+        <f>IF($A6=K$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.34722912450926274</v>
       </c>
       <c r="L6" s="5">
-        <f>IF($A6=L$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>10</v>
+        <f>IF($A6=L$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.34722912450926274</v>
       </c>
       <c r="M6" s="5">
-        <f>IF($A6=M$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>26</v>
+        <f>IF($A6=M$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.90279572372408312</v>
       </c>
       <c r="N6" s="5">
-        <f>IF($A6=N$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>28</v>
+        <f>IF($A6=N$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.9722415486259357</v>
       </c>
       <c r="O6" s="5">
-        <f>IF($A6=O$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>44</v>
+        <f>IF($A6=O$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.5278081478407561</v>
       </c>
       <c r="P6" s="5">
-        <f>IF($A6=P$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-6</v>
+        <f>IF($A6=P$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.20833747470555763</v>
       </c>
       <c r="Q6" s="5">
-        <f>IF($A6=Q$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A6=Q$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="R6" s="5">
-        <f>IF($A6=R$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-2</v>
+        <f>IF($A6=R$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-6.9445824901852582E-2</v>
       </c>
       <c r="S6" s="5">
-        <f>IF($A6=S$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>83</v>
+        <f>IF($A6=S$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.8820017334268808</v>
       </c>
       <c r="T6" s="5">
-        <f>IF($A6=T$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>60</v>
+        <f>IF($A6=T$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.0833747470555766</v>
       </c>
       <c r="U6" s="5">
-        <f>IF($A6=U$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-4</v>
+        <f>IF($A6=U$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.13889164980370516</v>
       </c>
       <c r="V6" s="5">
-        <f>IF($A6=V$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>11</v>
+        <f>IF($A6=V$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.38195203696018898</v>
       </c>
       <c r="W6" s="5">
-        <f>IF($A6=W$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>25</v>
+        <f>IF($A6=W$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.86807281127315683</v>
       </c>
       <c r="X6" s="5">
-        <f>IF($A6=X$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15.954545454545453</v>
+        <f>IF($A6=X$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55398828501250552</v>
       </c>
       <c r="Y6" s="5">
-        <f>IF($A6=Y$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-32</v>
+        <f>IF($A6=Y$1,VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A6,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1111331984296409</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
@@ -25279,100 +25376,100 @@
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <f>IF($A7=B$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A7=B$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027977</v>
       </c>
       <c r="C7" s="5">
-        <f>IF($A7=C$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>29</v>
+        <f>IF($A7=C$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.006964461076862</v>
       </c>
       <c r="D7" s="5">
-        <f>IF($A7=D$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A7=D$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="E7" s="5">
-        <f>IF($A7=E$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A7=E$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="F7" s="5">
-        <f>IF($A7=F$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-25</v>
+        <f>IF($A7=F$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.86807281127315683</v>
       </c>
       <c r="G7" s="5">
-        <f>IF($A7=G$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>128</v>
+        <f>IF($A7=G$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31408452626065136</v>
       </c>
       <c r="H7" s="5">
-        <f>IF($A7=H$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A7=H$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="I7" s="5">
-        <f>IF($A7=I$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-71</v>
+        <f>IF($A7=I$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.4653267840157653</v>
       </c>
       <c r="J7" s="5">
-        <f>IF($A7=J$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>9</v>
+        <f>IF($A7=J$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31250621205833645</v>
       </c>
       <c r="K7" s="5">
-        <f>IF($A7=K$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A7=K$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="L7" s="5">
-        <f>IF($A7=L$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A7=L$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="M7" s="5">
-        <f>IF($A7=M$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A7=M$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926291E-2</v>
       </c>
       <c r="N7" s="5">
-        <f>IF($A7=N$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>3</v>
+        <f>IF($A7=N$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.10416873735277882</v>
       </c>
       <c r="O7" s="5">
-        <f>IF($A7=O$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>19</v>
+        <f>IF($A7=O$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.65973533656759931</v>
       </c>
       <c r="P7" s="5">
-        <f>IF($A7=P$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-31</v>
+        <f>IF($A7=P$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0764102859787146</v>
       </c>
       <c r="Q7" s="5">
-        <f>IF($A7=Q$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-41</v>
+        <f>IF($A7=Q$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4236394104879773</v>
       </c>
       <c r="R7" s="5">
-        <f>IF($A7=R$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-27</v>
+        <f>IF($A7=R$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.93751863617500941</v>
       </c>
       <c r="S7" s="5">
-        <f>IF($A7=S$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>58</v>
+        <f>IF($A7=S$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.013928922153724</v>
       </c>
       <c r="T7" s="5">
-        <f>IF($A7=T$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>35</v>
+        <f>IF($A7=T$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.2153019357824197</v>
       </c>
       <c r="U7" s="5">
-        <f>IF($A7=U$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-29</v>
+        <f>IF($A7=U$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.006964461076862</v>
       </c>
       <c r="V7" s="5">
-        <f>IF($A7=V$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A7=V$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="W7" s="5">
-        <f>IF($A7=W$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A7=W$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="X7" s="5">
-        <f>IF($A7=X$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-9.0454545454545467</v>
+        <f>IF($A7=X$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.31408452626065136</v>
       </c>
       <c r="Y7" s="5">
-        <f>IF($A7=Y$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A7=Y$1,VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A7,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027977</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
@@ -25380,100 +25477,100 @@
         <v>6</v>
       </c>
       <c r="B8" s="5">
-        <f>IF($A8=B$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A8=B$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027977</v>
       </c>
       <c r="C8" s="5">
-        <f>IF($A8=C$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>29</v>
+        <f>IF($A8=C$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.006964461076862</v>
       </c>
       <c r="D8" s="5">
-        <f>IF($A8=D$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A8=D$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="E8" s="5">
-        <f>IF($A8=E$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A8=E$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="F8" s="5">
-        <f>IF($A8=F$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-25</v>
+        <f>IF($A8=F$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.86807281127315683</v>
       </c>
       <c r="G8" s="5">
-        <f>IF($A8=G$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A8=G$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="H8" s="5">
-        <f>IF($A8=H$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>128</v>
+        <f>IF($A8=H$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31408452626065136</v>
       </c>
       <c r="I8" s="5">
-        <f>IF($A8=I$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-71</v>
+        <f>IF($A8=I$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.4653267840157653</v>
       </c>
       <c r="J8" s="5">
-        <f>IF($A8=J$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>9</v>
+        <f>IF($A8=J$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31250621205833645</v>
       </c>
       <c r="K8" s="5">
-        <f>IF($A8=K$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A8=K$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="L8" s="5">
-        <f>IF($A8=L$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A8=L$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="M8" s="5">
-        <f>IF($A8=M$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A8=M$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926291E-2</v>
       </c>
       <c r="N8" s="5">
-        <f>IF($A8=N$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>3</v>
+        <f>IF($A8=N$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.10416873735277882</v>
       </c>
       <c r="O8" s="5">
-        <f>IF($A8=O$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>19</v>
+        <f>IF($A8=O$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.65973533656759931</v>
       </c>
       <c r="P8" s="5">
-        <f>IF($A8=P$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-31</v>
+        <f>IF($A8=P$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0764102859787146</v>
       </c>
       <c r="Q8" s="5">
-        <f>IF($A8=Q$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-41</v>
+        <f>IF($A8=Q$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4236394104879773</v>
       </c>
       <c r="R8" s="5">
-        <f>IF($A8=R$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-27</v>
+        <f>IF($A8=R$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.93751863617500941</v>
       </c>
       <c r="S8" s="5">
-        <f>IF($A8=S$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>58</v>
+        <f>IF($A8=S$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.013928922153724</v>
       </c>
       <c r="T8" s="5">
-        <f>IF($A8=T$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>35</v>
+        <f>IF($A8=T$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.2153019357824197</v>
       </c>
       <c r="U8" s="5">
-        <f>IF($A8=U$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-29</v>
+        <f>IF($A8=U$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.006964461076862</v>
       </c>
       <c r="V8" s="5">
-        <f>IF($A8=V$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A8=V$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="W8" s="5">
-        <f>IF($A8=W$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A8=W$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="X8" s="5">
-        <f>IF($A8=X$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-9.0454545454545467</v>
+        <f>IF($A8=X$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.31408452626065136</v>
       </c>
       <c r="Y8" s="5">
-        <f>IF($A8=Y$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A8=Y$1,VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A8,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027977</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -25481,100 +25578,100 @@
         <v>7</v>
       </c>
       <c r="B9" s="5">
-        <f>IF($A9=B$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A9=B$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296763</v>
       </c>
       <c r="C9" s="5">
-        <f>IF($A9=C$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>100</v>
+        <f>IF($A9=C$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926273</v>
       </c>
       <c r="D9" s="5">
-        <f>IF($A9=D$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A9=D$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027975</v>
       </c>
       <c r="E9" s="5">
-        <f>IF($A9=E$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A9=E$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027975</v>
       </c>
       <c r="F9" s="5">
-        <f>IF($A9=F$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>46</v>
+        <f>IF($A9=F$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.5972539727426085</v>
       </c>
       <c r="G9" s="5">
-        <f>IF($A9=G$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>71</v>
+        <f>IF($A9=G$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.4653267840157653</v>
       </c>
       <c r="H9" s="5">
-        <f>IF($A9=H$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>71</v>
+        <f>IF($A9=H$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.4653267840157653</v>
       </c>
       <c r="I9" s="5">
-        <f>IF($A9=I$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A9=I$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.151242257755114</v>
       </c>
       <c r="J9" s="5">
-        <f>IF($A9=J$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>80</v>
+        <f>IF($A9=J$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.7778329960741019</v>
       </c>
       <c r="K9" s="5">
-        <f>IF($A9=K$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>56</v>
+        <f>IF($A9=K$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9444830972518712</v>
       </c>
       <c r="L9" s="5">
-        <f>IF($A9=L$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>56</v>
+        <f>IF($A9=L$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9444830972518712</v>
       </c>
       <c r="M9" s="5">
-        <f>IF($A9=M$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>72</v>
+        <f>IF($A9=M$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.5000496964666916</v>
       </c>
       <c r="N9" s="5">
-        <f>IF($A9=N$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>74</v>
+        <f>IF($A9=N$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.5694955213685442</v>
       </c>
       <c r="O9" s="5">
-        <f>IF($A9=O$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>90</v>
+        <f>IF($A9=O$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.1250621205833644</v>
       </c>
       <c r="P9" s="5">
-        <f>IF($A9=P$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>40</v>
+        <f>IF($A9=P$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.3889164980370508</v>
       </c>
       <c r="Q9" s="5">
-        <f>IF($A9=Q$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>30</v>
+        <f>IF($A9=Q$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0416873735277881</v>
       </c>
       <c r="R9" s="5">
-        <f>IF($A9=R$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>44</v>
+        <f>IF($A9=R$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.5278081478407559</v>
       </c>
       <c r="S9" s="5">
-        <f>IF($A9=S$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>129</v>
+        <f>IF($A9=S$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>4.4792557061694893</v>
       </c>
       <c r="T9" s="5">
-        <f>IF($A9=T$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>106</v>
+        <f>IF($A9=T$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.6806287197981851</v>
       </c>
       <c r="U9" s="5">
-        <f>IF($A9=U$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>42</v>
+        <f>IF($A9=U$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4583623229389033</v>
       </c>
       <c r="V9" s="5">
-        <f>IF($A9=V$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A9=V$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027975</v>
       </c>
       <c r="W9" s="5">
-        <f>IF($A9=W$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>71</v>
+        <f>IF($A9=W$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.4653267840157653</v>
       </c>
       <c r="X9" s="5">
-        <f>IF($A9=X$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>61.954545454545453</v>
+        <f>IF($A9=X$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.151242257755114</v>
       </c>
       <c r="Y9" s="5">
-        <f>IF($A9=Y$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A9=Y$1,VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A9,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296763</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
@@ -25582,100 +25679,100 @@
         <v>8</v>
       </c>
       <c r="B10" s="5">
-        <f>IF($A10=B$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-66</v>
+        <f>IF($A10=B$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.2917122217611343</v>
       </c>
       <c r="C10" s="5">
-        <f>IF($A10=C$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>20</v>
+        <f>IF($A10=C$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.69445824901852549</v>
       </c>
       <c r="D10" s="5">
-        <f>IF($A10=D$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-23</v>
+        <f>IF($A10=D$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.79862698637130436</v>
       </c>
       <c r="E10" s="5">
-        <f>IF($A10=E$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-23</v>
+        <f>IF($A10=E$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.79862698637130436</v>
       </c>
       <c r="F10" s="5">
-        <f>IF($A10=F$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-34</v>
+        <f>IF($A10=F$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1805790233314934</v>
       </c>
       <c r="G10" s="5">
-        <f>IF($A10=G$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-9</v>
+        <f>IF($A10=G$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.31250621205833645</v>
       </c>
       <c r="H10" s="5">
-        <f>IF($A10=H$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-9</v>
+        <f>IF($A10=H$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.31250621205833645</v>
       </c>
       <c r="I10" s="5">
-        <f>IF($A10=I$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-80</v>
+        <f>IF($A10=I$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.7778329960741019</v>
       </c>
       <c r="J10" s="5">
-        <f>IF($A10=J$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>137</v>
+        <f>IF($A10=J$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.62659073831898782</v>
       </c>
       <c r="K10" s="5">
-        <f>IF($A10=K$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-24</v>
+        <f>IF($A10=K$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.83334989882223054</v>
       </c>
       <c r="L10" s="5">
-        <f>IF($A10=L$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-24</v>
+        <f>IF($A10=L$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.83334989882223054</v>
       </c>
       <c r="M10" s="5">
-        <f>IF($A10=M$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-8</v>
+        <f>IF($A10=M$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.27778329960741016</v>
       </c>
       <c r="N10" s="5">
-        <f>IF($A10=N$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-6</v>
+        <f>IF($A10=N$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.20833747470555763</v>
       </c>
       <c r="O10" s="5">
-        <f>IF($A10=O$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>10</v>
+        <f>IF($A10=O$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.3472291245092628</v>
       </c>
       <c r="P10" s="5">
-        <f>IF($A10=P$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-40</v>
+        <f>IF($A10=P$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.388916498037051</v>
       </c>
       <c r="Q10" s="5">
-        <f>IF($A10=Q$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-50</v>
+        <f>IF($A10=Q$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7361456225463137</v>
       </c>
       <c r="R10" s="5">
-        <f>IF($A10=R$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-36</v>
+        <f>IF($A10=R$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.250024848233346</v>
       </c>
       <c r="S10" s="5">
-        <f>IF($A10=S$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>49</v>
+        <f>IF($A10=S$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7014227100953874</v>
       </c>
       <c r="T10" s="5">
-        <f>IF($A10=T$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>26</v>
+        <f>IF($A10=T$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.90279572372408323</v>
       </c>
       <c r="U10" s="5">
-        <f>IF($A10=U$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-38</v>
+        <f>IF($A10=U$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.3194706731351986</v>
       </c>
       <c r="V10" s="5">
-        <f>IF($A10=V$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-23</v>
+        <f>IF($A10=V$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.79862698637130436</v>
       </c>
       <c r="W10" s="5">
-        <f>IF($A10=W$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-9</v>
+        <f>IF($A10=W$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.31250621205833645</v>
       </c>
       <c r="X10" s="5">
-        <f>IF($A10=X$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-18.045454545454547</v>
+        <f>IF($A10=X$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.62659073831898782</v>
       </c>
       <c r="Y10" s="5">
-        <f>IF($A10=Y$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-66</v>
+        <f>IF($A10=Y$1,VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A10,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.2917122217611343</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
@@ -25683,100 +25780,100 @@
         <v>9</v>
       </c>
       <c r="B11" s="5">
-        <f>IF($A11=B$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-42</v>
+        <f>IF($A11=B$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4583623229389036</v>
       </c>
       <c r="C11" s="5">
-        <f>IF($A11=C$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>44</v>
+        <f>IF($A11=C$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.5278081478407561</v>
       </c>
       <c r="D11" s="5">
-        <f>IF($A11=D$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A11=D$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926263E-2</v>
       </c>
       <c r="E11" s="5">
-        <f>IF($A11=E$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A11=E$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926263E-2</v>
       </c>
       <c r="F11" s="5">
-        <f>IF($A11=F$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-10</v>
+        <f>IF($A11=F$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.34722912450926274</v>
       </c>
       <c r="G11" s="5">
-        <f>IF($A11=G$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A11=G$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="H11" s="5">
-        <f>IF($A11=H$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A11=H$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="I11" s="5">
-        <f>IF($A11=I$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-56</v>
+        <f>IF($A11=I$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9444830972518712</v>
       </c>
       <c r="J11" s="5">
-        <f>IF($A11=J$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>24</v>
+        <f>IF($A11=J$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.83334989882223054</v>
       </c>
       <c r="K11" s="5">
-        <f>IF($A11=K$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>113</v>
+        <f>IF($A11=K$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.20675916050324278</v>
       </c>
       <c r="L11" s="5">
-        <f>IF($A11=L$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A11=L$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="M11" s="5">
-        <f>IF($A11=M$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A11=M$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="N11" s="5">
-        <f>IF($A11=N$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>18</v>
+        <f>IF($A11=N$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.62501242411667302</v>
       </c>
       <c r="O11" s="5">
-        <f>IF($A11=O$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>34</v>
+        <f>IF($A11=O$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1805790233314934</v>
       </c>
       <c r="P11" s="5">
-        <f>IF($A11=P$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A11=P$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="Q11" s="5">
-        <f>IF($A11=Q$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-26</v>
+        <f>IF($A11=Q$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.90279572372408312</v>
       </c>
       <c r="R11" s="5">
-        <f>IF($A11=R$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-12</v>
+        <f>IF($A11=R$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.41667494941111533</v>
       </c>
       <c r="S11" s="5">
-        <f>IF($A11=S$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>73</v>
+        <f>IF($A11=S$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.5347726089176179</v>
       </c>
       <c r="T11" s="5">
-        <f>IF($A11=T$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>50</v>
+        <f>IF($A11=T$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7361456225463139</v>
       </c>
       <c r="U11" s="5">
-        <f>IF($A11=U$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A11=U$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296791</v>
       </c>
       <c r="V11" s="5">
-        <f>IF($A11=V$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A11=V$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926263E-2</v>
       </c>
       <c r="W11" s="5">
-        <f>IF($A11=W$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A11=W$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="X11" s="5">
-        <f>IF($A11=X$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>5.9545454545454533</v>
+        <f>IF($A11=X$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.20675916050324278</v>
       </c>
       <c r="Y11" s="5">
-        <f>IF($A11=Y$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-42</v>
+        <f>IF($A11=Y$1,VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A11,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4583623229389036</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
@@ -25784,100 +25881,100 @@
         <v>10</v>
       </c>
       <c r="B12" s="5">
-        <f>IF($A12=B$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-42</v>
+        <f>IF($A12=B$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4583623229389036</v>
       </c>
       <c r="C12" s="5">
-        <f>IF($A12=C$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>44</v>
+        <f>IF($A12=C$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.5278081478407561</v>
       </c>
       <c r="D12" s="5">
-        <f>IF($A12=D$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A12=D$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926263E-2</v>
       </c>
       <c r="E12" s="5">
-        <f>IF($A12=E$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A12=E$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926263E-2</v>
       </c>
       <c r="F12" s="5">
-        <f>IF($A12=F$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-10</v>
+        <f>IF($A12=F$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.34722912450926274</v>
       </c>
       <c r="G12" s="5">
-        <f>IF($A12=G$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A12=G$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="H12" s="5">
-        <f>IF($A12=H$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A12=H$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="I12" s="5">
-        <f>IF($A12=I$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-56</v>
+        <f>IF($A12=I$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9444830972518712</v>
       </c>
       <c r="J12" s="5">
-        <f>IF($A12=J$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>24</v>
+        <f>IF($A12=J$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.83334989882223054</v>
       </c>
       <c r="K12" s="5">
-        <f>IF($A12=K$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A12=K$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="L12" s="5">
-        <f>IF($A12=L$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>113</v>
+        <f>IF($A12=L$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.20675916050324278</v>
       </c>
       <c r="M12" s="5">
-        <f>IF($A12=M$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A12=M$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="N12" s="5">
-        <f>IF($A12=N$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>18</v>
+        <f>IF($A12=N$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.62501242411667302</v>
       </c>
       <c r="O12" s="5">
-        <f>IF($A12=O$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>34</v>
+        <f>IF($A12=O$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1805790233314934</v>
       </c>
       <c r="P12" s="5">
-        <f>IF($A12=P$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A12=P$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="Q12" s="5">
-        <f>IF($A12=Q$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-26</v>
+        <f>IF($A12=Q$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.90279572372408312</v>
       </c>
       <c r="R12" s="5">
-        <f>IF($A12=R$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-12</v>
+        <f>IF($A12=R$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.41667494941111533</v>
       </c>
       <c r="S12" s="5">
-        <f>IF($A12=S$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>73</v>
+        <f>IF($A12=S$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.5347726089176179</v>
       </c>
       <c r="T12" s="5">
-        <f>IF($A12=T$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>50</v>
+        <f>IF($A12=T$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7361456225463139</v>
       </c>
       <c r="U12" s="5">
-        <f>IF($A12=U$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A12=U$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296791</v>
       </c>
       <c r="V12" s="5">
-        <f>IF($A12=V$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A12=V$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926263E-2</v>
       </c>
       <c r="W12" s="5">
-        <f>IF($A12=W$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A12=W$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="X12" s="5">
-        <f>IF($A12=X$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>5.9545454545454533</v>
+        <f>IF($A12=X$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.20675916050324278</v>
       </c>
       <c r="Y12" s="5">
-        <f>IF($A12=Y$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-42</v>
+        <f>IF($A12=Y$1,VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A12,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4583623229389036</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
@@ -25885,100 +25982,100 @@
         <v>11</v>
       </c>
       <c r="B13" s="5">
-        <f>IF($A13=B$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-58</v>
+        <f>IF($A13=B$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.013928922153724</v>
       </c>
       <c r="C13" s="5">
-        <f>IF($A13=C$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>28</v>
+        <f>IF($A13=C$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.9722415486259357</v>
       </c>
       <c r="D13" s="5">
-        <f>IF($A13=D$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A13=D$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="E13" s="5">
-        <f>IF($A13=E$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A13=E$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="F13" s="5">
-        <f>IF($A13=F$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-26</v>
+        <f>IF($A13=F$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.90279572372408312</v>
       </c>
       <c r="G13" s="5">
-        <f>IF($A13=G$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A13=G$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926291E-2</v>
       </c>
       <c r="H13" s="5">
-        <f>IF($A13=H$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A13=H$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926291E-2</v>
       </c>
       <c r="I13" s="5">
-        <f>IF($A13=I$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-72</v>
+        <f>IF($A13=I$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.5000496964666916</v>
       </c>
       <c r="J13" s="5">
-        <f>IF($A13=J$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>8</v>
+        <f>IF($A13=J$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.27778329960741016</v>
       </c>
       <c r="K13" s="5">
-        <f>IF($A13=K$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A13=K$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="L13" s="5">
-        <f>IF($A13=L$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A13=L$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="M13" s="5">
-        <f>IF($A13=M$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>129</v>
+        <f>IF($A13=M$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.34880743871157766</v>
       </c>
       <c r="N13" s="5">
-        <f>IF($A13=N$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>2</v>
+        <f>IF($A13=N$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>6.9445824901852526E-2</v>
       </c>
       <c r="O13" s="5">
-        <f>IF($A13=O$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>18</v>
+        <f>IF($A13=O$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.62501242411667302</v>
       </c>
       <c r="P13" s="5">
-        <f>IF($A13=P$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-32</v>
+        <f>IF($A13=P$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1111331984296409</v>
       </c>
       <c r="Q13" s="5">
-        <f>IF($A13=Q$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-42</v>
+        <f>IF($A13=Q$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4583623229389036</v>
       </c>
       <c r="R13" s="5">
-        <f>IF($A13=R$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-28</v>
+        <f>IF($A13=R$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.9722415486259357</v>
       </c>
       <c r="S13" s="5">
-        <f>IF($A13=S$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A13=S$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027977</v>
       </c>
       <c r="T13" s="5">
-        <f>IF($A13=T$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>34</v>
+        <f>IF($A13=T$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1805790233314934</v>
       </c>
       <c r="U13" s="5">
-        <f>IF($A13=U$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-30</v>
+        <f>IF($A13=U$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0416873735277883</v>
       </c>
       <c r="V13" s="5">
-        <f>IF($A13=V$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A13=V$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="W13" s="5">
-        <f>IF($A13=W$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A13=W$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926291E-2</v>
       </c>
       <c r="X13" s="5">
-        <f>IF($A13=X$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-10.045454545454547</v>
+        <f>IF($A13=X$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.34880743871157766</v>
       </c>
       <c r="Y13" s="5">
-        <f>IF($A13=Y$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-58</v>
+        <f>IF($A13=Y$1,VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A13,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.013928922153724</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
@@ -25986,100 +26083,100 @@
         <v>12</v>
       </c>
       <c r="B14" s="5">
-        <f>IF($A14=B$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-60</v>
+        <f>IF($A14=B$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.0833747470555766</v>
       </c>
       <c r="C14" s="5">
-        <f>IF($A14=C$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>26</v>
+        <f>IF($A14=C$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.90279572372408312</v>
       </c>
       <c r="D14" s="5">
-        <f>IF($A14=D$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-17</v>
+        <f>IF($A14=D$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.59028951166574672</v>
       </c>
       <c r="E14" s="5">
-        <f>IF($A14=E$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-17</v>
+        <f>IF($A14=E$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.59028951166574672</v>
       </c>
       <c r="F14" s="5">
-        <f>IF($A14=F$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-28</v>
+        <f>IF($A14=F$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.9722415486259357</v>
       </c>
       <c r="G14" s="5">
-        <f>IF($A14=G$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-3</v>
+        <f>IF($A14=G$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.10416873735277882</v>
       </c>
       <c r="H14" s="5">
-        <f>IF($A14=H$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-3</v>
+        <f>IF($A14=H$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.10416873735277882</v>
       </c>
       <c r="I14" s="5">
-        <f>IF($A14=I$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-74</v>
+        <f>IF($A14=I$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.5694955213685442</v>
       </c>
       <c r="J14" s="5">
-        <f>IF($A14=J$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>6</v>
+        <f>IF($A14=J$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.20833747470555763</v>
       </c>
       <c r="K14" s="5">
-        <f>IF($A14=K$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-18</v>
+        <f>IF($A14=K$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.62501242411667302</v>
       </c>
       <c r="L14" s="5">
-        <f>IF($A14=L$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-18</v>
+        <f>IF($A14=L$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.62501242411667302</v>
       </c>
       <c r="M14" s="5">
-        <f>IF($A14=M$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-2</v>
+        <f>IF($A14=M$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-6.9445824901852526E-2</v>
       </c>
       <c r="N14" s="5">
-        <f>IF($A14=N$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>131</v>
+        <f>IF($A14=N$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.41825326361343018</v>
       </c>
       <c r="O14" s="5">
-        <f>IF($A14=O$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A14=O$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="P14" s="5">
-        <f>IF($A14=P$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-34</v>
+        <f>IF($A14=P$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1805790233314934</v>
       </c>
       <c r="Q14" s="5">
-        <f>IF($A14=Q$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-44</v>
+        <f>IF($A14=Q$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.5278081478407561</v>
       </c>
       <c r="R14" s="5">
-        <f>IF($A14=R$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-30</v>
+        <f>IF($A14=R$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0416873735277883</v>
       </c>
       <c r="S14" s="5">
-        <f>IF($A14=S$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>55</v>
+        <f>IF($A14=S$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9097601848009451</v>
       </c>
       <c r="T14" s="5">
-        <f>IF($A14=T$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>32</v>
+        <f>IF($A14=T$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1111331984296409</v>
       </c>
       <c r="U14" s="5">
-        <f>IF($A14=U$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-32</v>
+        <f>IF($A14=U$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1111331984296409</v>
       </c>
       <c r="V14" s="5">
-        <f>IF($A14=V$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-17</v>
+        <f>IF($A14=V$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.59028951166574672</v>
       </c>
       <c r="W14" s="5">
-        <f>IF($A14=W$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-3</v>
+        <f>IF($A14=W$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.10416873735277882</v>
       </c>
       <c r="X14" s="5">
-        <f>IF($A14=X$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-12.045454545454547</v>
+        <f>IF($A14=X$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.41825326361343018</v>
       </c>
       <c r="Y14" s="5">
-        <f>IF($A14=Y$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-60</v>
+        <f>IF($A14=Y$1,VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A14,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.0833747470555766</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
@@ -26087,100 +26184,100 @@
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <f>IF($A15=B$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-76</v>
+        <f>IF($A15=B$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.6389413462703972</v>
       </c>
       <c r="C15" s="5">
-        <f>IF($A15=C$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>10</v>
+        <f>IF($A15=C$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.34722912450926269</v>
       </c>
       <c r="D15" s="5">
-        <f>IF($A15=D$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-33</v>
+        <f>IF($A15=D$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1458561108805672</v>
       </c>
       <c r="E15" s="5">
-        <f>IF($A15=E$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-33</v>
+        <f>IF($A15=E$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1458561108805672</v>
       </c>
       <c r="F15" s="5">
-        <f>IF($A15=F$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-44</v>
+        <f>IF($A15=F$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.5278081478407561</v>
       </c>
       <c r="G15" s="5">
-        <f>IF($A15=G$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-19</v>
+        <f>IF($A15=G$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.65973533656759931</v>
       </c>
       <c r="H15" s="5">
-        <f>IF($A15=H$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-19</v>
+        <f>IF($A15=H$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.65973533656759931</v>
       </c>
       <c r="I15" s="5">
-        <f>IF($A15=I$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-90</v>
+        <f>IF($A15=I$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.1250621205833644</v>
       </c>
       <c r="J15" s="5">
-        <f>IF($A15=J$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-10</v>
+        <f>IF($A15=J$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.3472291245092628</v>
       </c>
       <c r="K15" s="5">
-        <f>IF($A15=K$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-34</v>
+        <f>IF($A15=K$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1805790233314934</v>
       </c>
       <c r="L15" s="5">
-        <f>IF($A15=L$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-34</v>
+        <f>IF($A15=L$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1805790233314934</v>
       </c>
       <c r="M15" s="5">
-        <f>IF($A15=M$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-18</v>
+        <f>IF($A15=M$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.62501242411667302</v>
       </c>
       <c r="N15" s="5">
-        <f>IF($A15=N$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A15=N$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="O15" s="5">
-        <f>IF($A15=O$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>147</v>
+        <f>IF($A15=O$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.97381986282825062</v>
       </c>
       <c r="P15" s="5">
-        <f>IF($A15=P$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-50</v>
+        <f>IF($A15=P$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7361456225463137</v>
       </c>
       <c r="Q15" s="5">
-        <f>IF($A15=Q$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-60</v>
+        <f>IF($A15=Q$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.0833747470555766</v>
       </c>
       <c r="R15" s="5">
-        <f>IF($A15=R$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-46</v>
+        <f>IF($A15=R$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.5972539727426087</v>
       </c>
       <c r="S15" s="5">
-        <f>IF($A15=S$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>39</v>
+        <f>IF($A15=S$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.3541935855861247</v>
       </c>
       <c r="T15" s="5">
-        <f>IF($A15=T$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A15=T$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="U15" s="5">
-        <f>IF($A15=U$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-48</v>
+        <f>IF($A15=U$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.6666997976444613</v>
       </c>
       <c r="V15" s="5">
-        <f>IF($A15=V$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-33</v>
+        <f>IF($A15=V$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1458561108805672</v>
       </c>
       <c r="W15" s="5">
-        <f>IF($A15=W$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-19</v>
+        <f>IF($A15=W$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.65973533656759931</v>
       </c>
       <c r="X15" s="5">
-        <f>IF($A15=X$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-28.045454545454547</v>
+        <f>IF($A15=X$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.97381986282825062</v>
       </c>
       <c r="Y15" s="5">
-        <f>IF($A15=Y$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-76</v>
+        <f>IF($A15=Y$1,VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A15,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.6389413462703972</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
@@ -26188,100 +26285,100 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <f>IF($A16=B$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-26</v>
+        <f>IF($A16=B$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.90279572372408323</v>
       </c>
       <c r="C16" s="5">
-        <f>IF($A16=C$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>60</v>
+        <f>IF($A16=C$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.0833747470555766</v>
       </c>
       <c r="D16" s="5">
-        <f>IF($A16=D$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>17</v>
+        <f>IF($A16=D$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.59028951166574661</v>
       </c>
       <c r="E16" s="5">
-        <f>IF($A16=E$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>17</v>
+        <f>IF($A16=E$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.59028951166574661</v>
       </c>
       <c r="F16" s="5">
-        <f>IF($A16=F$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>6</v>
+        <f>IF($A16=F$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.20833747470555763</v>
       </c>
       <c r="G16" s="5">
-        <f>IF($A16=G$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>31</v>
+        <f>IF($A16=G$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0764102859787146</v>
       </c>
       <c r="H16" s="5">
-        <f>IF($A16=H$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>31</v>
+        <f>IF($A16=H$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0764102859787146</v>
       </c>
       <c r="I16" s="5">
-        <f>IF($A16=I$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-40</v>
+        <f>IF($A16=I$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.3889164980370508</v>
       </c>
       <c r="J16" s="5">
-        <f>IF($A16=J$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>40</v>
+        <f>IF($A16=J$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.388916498037051</v>
       </c>
       <c r="K16" s="5">
-        <f>IF($A16=K$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A16=K$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="L16" s="5">
-        <f>IF($A16=L$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A16=L$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="M16" s="5">
-        <f>IF($A16=M$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>32</v>
+        <f>IF($A16=M$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1111331984296409</v>
       </c>
       <c r="N16" s="5">
-        <f>IF($A16=N$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>34</v>
+        <f>IF($A16=N$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1805790233314934</v>
       </c>
       <c r="O16" s="5">
-        <f>IF($A16=O$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>50</v>
+        <f>IF($A16=O$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7361456225463137</v>
       </c>
       <c r="P16" s="5">
-        <f>IF($A16=P$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>97</v>
+        <f>IF($A16=P$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.76232575971806316</v>
       </c>
       <c r="Q16" s="5">
-        <f>IF($A16=Q$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-10</v>
+        <f>IF($A16=Q$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.3472291245092628</v>
       </c>
       <c r="R16" s="5">
-        <f>IF($A16=R$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>4</v>
+        <f>IF($A16=R$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.13889164980370505</v>
       </c>
       <c r="S16" s="5">
-        <f>IF($A16=S$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>89</v>
+        <f>IF($A16=S$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.0903392081324386</v>
       </c>
       <c r="T16" s="5">
-        <f>IF($A16=T$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>66</v>
+        <f>IF($A16=T$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.2917122217611343</v>
       </c>
       <c r="U16" s="5">
-        <f>IF($A16=U$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>2</v>
+        <f>IF($A16=U$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>6.9445824901852471E-2</v>
       </c>
       <c r="V16" s="5">
-        <f>IF($A16=V$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>17</v>
+        <f>IF($A16=V$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.59028951166574661</v>
       </c>
       <c r="W16" s="5">
-        <f>IF($A16=W$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>31</v>
+        <f>IF($A16=W$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0764102859787146</v>
       </c>
       <c r="X16" s="5">
-        <f>IF($A16=X$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>21.954545454545453</v>
+        <f>IF($A16=X$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.76232575971806316</v>
       </c>
       <c r="Y16" s="5">
-        <f>IF($A16=Y$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-26</v>
+        <f>IF($A16=Y$1,VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A16,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.90279572372408323</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
@@ -26289,100 +26386,100 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <f>IF($A17=B$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A17=B$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="C17" s="5">
-        <f>IF($A17=C$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>70</v>
+        <f>IF($A17=C$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.4306038715648395</v>
       </c>
       <c r="D17" s="5">
-        <f>IF($A17=D$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>27</v>
+        <f>IF($A17=D$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.93751863617500941</v>
       </c>
       <c r="E17" s="5">
-        <f>IF($A17=E$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>27</v>
+        <f>IF($A17=E$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.93751863617500941</v>
       </c>
       <c r="F17" s="5">
-        <f>IF($A17=F$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A17=F$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="G17" s="5">
-        <f>IF($A17=G$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>41</v>
+        <f>IF($A17=G$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4236394104879773</v>
       </c>
       <c r="H17" s="5">
-        <f>IF($A17=H$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>41</v>
+        <f>IF($A17=H$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4236394104879773</v>
       </c>
       <c r="I17" s="5">
-        <f>IF($A17=I$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-30</v>
+        <f>IF($A17=I$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0416873735277881</v>
       </c>
       <c r="J17" s="5">
-        <f>IF($A17=J$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>50</v>
+        <f>IF($A17=J$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7361456225463137</v>
       </c>
       <c r="K17" s="5">
-        <f>IF($A17=K$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>26</v>
+        <f>IF($A17=K$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.90279572372408312</v>
       </c>
       <c r="L17" s="5">
-        <f>IF($A17=L$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>26</v>
+        <f>IF($A17=L$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.90279572372408312</v>
       </c>
       <c r="M17" s="5">
-        <f>IF($A17=M$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>42</v>
+        <f>IF($A17=M$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4583623229389036</v>
       </c>
       <c r="N17" s="5">
-        <f>IF($A17=N$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>44</v>
+        <f>IF($A17=N$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.5278081478407561</v>
       </c>
       <c r="O17" s="5">
-        <f>IF($A17=O$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>60</v>
+        <f>IF($A17=O$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.0833747470555766</v>
       </c>
       <c r="P17" s="5">
-        <f>IF($A17=P$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>10</v>
+        <f>IF($A17=P$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.3472291245092628</v>
       </c>
       <c r="Q17" s="5">
-        <f>IF($A17=Q$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>87</v>
+        <f>IF($A17=Q$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.109554884227326</v>
       </c>
       <c r="R17" s="5">
-        <f>IF($A17=R$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A17=R$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="S17" s="5">
-        <f>IF($A17=S$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>99</v>
+        <f>IF($A17=S$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4375683326417015</v>
       </c>
       <c r="T17" s="5">
-        <f>IF($A17=T$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>76</v>
+        <f>IF($A17=T$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.6389413462703972</v>
       </c>
       <c r="U17" s="5">
-        <f>IF($A17=U$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>12</v>
+        <f>IF($A17=U$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.41667494941111527</v>
       </c>
       <c r="V17" s="5">
-        <f>IF($A17=V$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>27</v>
+        <f>IF($A17=V$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.93751863617500941</v>
       </c>
       <c r="W17" s="5">
-        <f>IF($A17=W$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>41</v>
+        <f>IF($A17=W$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4236394104879773</v>
       </c>
       <c r="X17" s="5">
-        <f>IF($A17=X$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>31.954545454545453</v>
+        <f>IF($A17=X$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.109554884227326</v>
       </c>
       <c r="Y17" s="5">
-        <f>IF($A17=Y$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A17=Y$1,VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A17,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
@@ -26390,100 +26487,100 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <f>IF($A18=B$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-30</v>
+        <f>IF($A18=B$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0416873735277883</v>
       </c>
       <c r="C18" s="5">
-        <f>IF($A18=C$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>56</v>
+        <f>IF($A18=C$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9444830972518714</v>
       </c>
       <c r="D18" s="5">
-        <f>IF($A18=D$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>13</v>
+        <f>IF($A18=D$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.45139786186204156</v>
       </c>
       <c r="E18" s="5">
-        <f>IF($A18=E$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>13</v>
+        <f>IF($A18=E$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.45139786186204156</v>
       </c>
       <c r="F18" s="5">
-        <f>IF($A18=F$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>2</v>
+        <f>IF($A18=F$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>6.9445824901852582E-2</v>
       </c>
       <c r="G18" s="5">
-        <f>IF($A18=G$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>27</v>
+        <f>IF($A18=G$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.93751863617500941</v>
       </c>
       <c r="H18" s="5">
-        <f>IF($A18=H$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>27</v>
+        <f>IF($A18=H$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.93751863617500941</v>
       </c>
       <c r="I18" s="5">
-        <f>IF($A18=I$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-44</v>
+        <f>IF($A18=I$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.5278081478407559</v>
       </c>
       <c r="J18" s="5">
-        <f>IF($A18=J$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>36</v>
+        <f>IF($A18=J$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.250024848233346</v>
       </c>
       <c r="K18" s="5">
-        <f>IF($A18=K$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>12</v>
+        <f>IF($A18=K$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.41667494941111533</v>
       </c>
       <c r="L18" s="5">
-        <f>IF($A18=L$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>12</v>
+        <f>IF($A18=L$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.41667494941111533</v>
       </c>
       <c r="M18" s="5">
-        <f>IF($A18=M$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>28</v>
+        <f>IF($A18=M$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.9722415486259357</v>
       </c>
       <c r="N18" s="5">
-        <f>IF($A18=N$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>30</v>
+        <f>IF($A18=N$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0416873735277883</v>
       </c>
       <c r="O18" s="5">
-        <f>IF($A18=O$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>46</v>
+        <f>IF($A18=O$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.5972539727426087</v>
       </c>
       <c r="P18" s="5">
-        <f>IF($A18=P$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-4</v>
+        <f>IF($A18=P$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.13889164980370505</v>
       </c>
       <c r="Q18" s="5">
-        <f>IF($A18=Q$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A18=Q$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="R18" s="5">
-        <f>IF($A18=R$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>101</v>
+        <f>IF($A18=R$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.6234341099143581</v>
       </c>
       <c r="S18" s="5">
-        <f>IF($A18=S$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>85</v>
+        <f>IF($A18=S$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.9514475583287334</v>
       </c>
       <c r="T18" s="5">
-        <f>IF($A18=T$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>62</v>
+        <f>IF($A18=T$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.1528205719574292</v>
       </c>
       <c r="U18" s="5">
-        <f>IF($A18=U$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-2</v>
+        <f>IF($A18=U$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-6.9445824901852582E-2</v>
       </c>
       <c r="V18" s="5">
-        <f>IF($A18=V$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>13</v>
+        <f>IF($A18=V$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.45139786186204156</v>
       </c>
       <c r="W18" s="5">
-        <f>IF($A18=W$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>27</v>
+        <f>IF($A18=W$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.93751863617500941</v>
       </c>
       <c r="X18" s="5">
-        <f>IF($A18=X$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>17.954545454545453</v>
+        <f>IF($A18=X$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.6234341099143581</v>
       </c>
       <c r="Y18" s="5">
-        <f>IF($A18=Y$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-30</v>
+        <f>IF($A18=Y$1,VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A18,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0416873735277883</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
@@ -26491,100 +26588,100 @@
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <f>IF($A19=B$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-115</v>
+        <f>IF($A19=B$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.9931349318565217</v>
       </c>
       <c r="C19" s="5">
-        <f>IF($A19=C$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-29</v>
+        <f>IF($A19=C$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.006964461076862</v>
       </c>
       <c r="D19" s="5">
-        <f>IF($A19=D$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-72</v>
+        <f>IF($A19=D$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.5000496964666916</v>
       </c>
       <c r="E19" s="5">
-        <f>IF($A19=E$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-72</v>
+        <f>IF($A19=E$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.5000496964666916</v>
       </c>
       <c r="F19" s="5">
-        <f>IF($A19=F$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-83</v>
+        <f>IF($A19=F$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.8820017334268808</v>
       </c>
       <c r="G19" s="5">
-        <f>IF($A19=G$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-58</v>
+        <f>IF($A19=G$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.013928922153724</v>
       </c>
       <c r="H19" s="5">
-        <f>IF($A19=H$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-58</v>
+        <f>IF($A19=H$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.013928922153724</v>
       </c>
       <c r="I19" s="5">
-        <f>IF($A19=I$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-129</v>
+        <f>IF($A19=I$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-4.4792557061694893</v>
       </c>
       <c r="J19" s="5">
-        <f>IF($A19=J$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-49</v>
+        <f>IF($A19=J$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7014227100953874</v>
       </c>
       <c r="K19" s="5">
-        <f>IF($A19=K$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-73</v>
+        <f>IF($A19=K$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.5347726089176179</v>
       </c>
       <c r="L19" s="5">
-        <f>IF($A19=L$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-73</v>
+        <f>IF($A19=L$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.5347726089176179</v>
       </c>
       <c r="M19" s="5">
-        <f>IF($A19=M$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A19=M$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027977</v>
       </c>
       <c r="N19" s="5">
-        <f>IF($A19=N$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-55</v>
+        <f>IF($A19=N$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9097601848009451</v>
       </c>
       <c r="O19" s="5">
-        <f>IF($A19=O$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-39</v>
+        <f>IF($A19=O$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.3541935855861247</v>
       </c>
       <c r="P19" s="5">
-        <f>IF($A19=P$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-89</v>
+        <f>IF($A19=P$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.0903392081324386</v>
       </c>
       <c r="Q19" s="5">
-        <f>IF($A19=Q$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-99</v>
+        <f>IF($A19=Q$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4375683326417015</v>
       </c>
       <c r="R19" s="5">
-        <f>IF($A19=R$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-85</v>
+        <f>IF($A19=R$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.9514475583287334</v>
       </c>
       <c r="S19" s="5">
-        <f>IF($A19=S$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>186</v>
+        <f>IF($A19=S$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.3280134484143753</v>
       </c>
       <c r="T19" s="5">
-        <f>IF($A19=T$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-23</v>
+        <f>IF($A19=T$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.79862698637130425</v>
       </c>
       <c r="U19" s="5">
-        <f>IF($A19=U$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-87</v>
+        <f>IF($A19=U$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.020893383230586</v>
       </c>
       <c r="V19" s="5">
-        <f>IF($A19=V$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-72</v>
+        <f>IF($A19=V$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.5000496964666916</v>
       </c>
       <c r="W19" s="5">
-        <f>IF($A19=W$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-58</v>
+        <f>IF($A19=W$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.013928922153724</v>
       </c>
       <c r="X19" s="5">
-        <f>IF($A19=X$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-67.045454545454547</v>
+        <f>IF($A19=X$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.3280134484143753</v>
       </c>
       <c r="Y19" s="5">
-        <f>IF($A19=Y$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-115</v>
+        <f>IF($A19=Y$1,VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A19,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.9931349318565217</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
@@ -26592,100 +26689,100 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <f>IF($A20=B$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-92</v>
+        <f>IF($A20=B$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.1945079454852174</v>
       </c>
       <c r="C20" s="5">
-        <f>IF($A20=C$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-6</v>
+        <f>IF($A20=C$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.20833747470555775</v>
       </c>
       <c r="D20" s="5">
-        <f>IF($A20=D$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-49</v>
+        <f>IF($A20=D$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7014227100953876</v>
       </c>
       <c r="E20" s="5">
-        <f>IF($A20=E$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-49</v>
+        <f>IF($A20=E$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7014227100953876</v>
       </c>
       <c r="F20" s="5">
-        <f>IF($A20=F$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-60</v>
+        <f>IF($A20=F$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.0833747470555766</v>
       </c>
       <c r="G20" s="5">
-        <f>IF($A20=G$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-35</v>
+        <f>IF($A20=G$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.2153019357824197</v>
       </c>
       <c r="H20" s="5">
-        <f>IF($A20=H$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-35</v>
+        <f>IF($A20=H$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.2153019357824197</v>
       </c>
       <c r="I20" s="5">
-        <f>IF($A20=I$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-106</v>
+        <f>IF($A20=I$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.6806287197981851</v>
       </c>
       <c r="J20" s="5">
-        <f>IF($A20=J$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-26</v>
+        <f>IF($A20=J$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.90279572372408323</v>
       </c>
       <c r="K20" s="5">
-        <f>IF($A20=K$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-50</v>
+        <f>IF($A20=K$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7361456225463139</v>
       </c>
       <c r="L20" s="5">
-        <f>IF($A20=L$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-50</v>
+        <f>IF($A20=L$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7361456225463139</v>
       </c>
       <c r="M20" s="5">
-        <f>IF($A20=M$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-34</v>
+        <f>IF($A20=M$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1805790233314934</v>
       </c>
       <c r="N20" s="5">
-        <f>IF($A20=N$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-32</v>
+        <f>IF($A20=N$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.1111331984296409</v>
       </c>
       <c r="O20" s="5">
-        <f>IF($A20=O$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-16</v>
+        <f>IF($A20=O$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55556659921482043</v>
       </c>
       <c r="P20" s="5">
-        <f>IF($A20=P$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-66</v>
+        <f>IF($A20=P$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.2917122217611343</v>
       </c>
       <c r="Q20" s="5">
-        <f>IF($A20=Q$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-76</v>
+        <f>IF($A20=Q$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.6389413462703972</v>
       </c>
       <c r="R20" s="5">
-        <f>IF($A20=R$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-62</v>
+        <f>IF($A20=R$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.1528205719574292</v>
       </c>
       <c r="S20" s="5">
-        <f>IF($A20=S$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>23</v>
+        <f>IF($A20=S$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.79862698637130425</v>
       </c>
       <c r="T20" s="5">
-        <f>IF($A20=T$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>163</v>
+        <f>IF($A20=T$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.529386462043071</v>
       </c>
       <c r="U20" s="5">
-        <f>IF($A20=U$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-64</v>
+        <f>IF($A20=U$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.2222663968592817</v>
       </c>
       <c r="V20" s="5">
-        <f>IF($A20=V$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-49</v>
+        <f>IF($A20=V$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.7014227100953876</v>
       </c>
       <c r="W20" s="5">
-        <f>IF($A20=W$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-35</v>
+        <f>IF($A20=W$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.2153019357824197</v>
       </c>
       <c r="X20" s="5">
-        <f>IF($A20=X$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-44.045454545454547</v>
+        <f>IF($A20=X$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.529386462043071</v>
       </c>
       <c r="Y20" s="5">
-        <f>IF($A20=Y$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-92</v>
+        <f>IF($A20=Y$1,VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A20,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.1945079454852174</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
@@ -26693,100 +26790,100 @@
         <v>19</v>
       </c>
       <c r="B21" s="5">
-        <f>IF($A21=B$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-28</v>
+        <f>IF($A21=B$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.9722415486259357</v>
       </c>
       <c r="C21" s="5">
-        <f>IF($A21=C$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>58</v>
+        <f>IF($A21=C$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.013928922153724</v>
       </c>
       <c r="D21" s="5">
-        <f>IF($A21=D$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A21=D$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="E21" s="5">
-        <f>IF($A21=E$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A21=E$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="F21" s="5">
-        <f>IF($A21=F$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>4</v>
+        <f>IF($A21=F$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.13889164980370516</v>
       </c>
       <c r="G21" s="5">
-        <f>IF($A21=G$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>29</v>
+        <f>IF($A21=G$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.006964461076862</v>
       </c>
       <c r="H21" s="5">
-        <f>IF($A21=H$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>29</v>
+        <f>IF($A21=H$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.006964461076862</v>
       </c>
       <c r="I21" s="5">
-        <f>IF($A21=I$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-42</v>
+        <f>IF($A21=I$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4583623229389033</v>
       </c>
       <c r="J21" s="5">
-        <f>IF($A21=J$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>38</v>
+        <f>IF($A21=J$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.3194706731351986</v>
       </c>
       <c r="K21" s="5">
-        <f>IF($A21=K$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A21=K$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296791</v>
       </c>
       <c r="L21" s="5">
-        <f>IF($A21=L$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A21=L$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296791</v>
       </c>
       <c r="M21" s="5">
-        <f>IF($A21=M$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>30</v>
+        <f>IF($A21=M$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0416873735277883</v>
       </c>
       <c r="N21" s="5">
-        <f>IF($A21=N$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>32</v>
+        <f>IF($A21=N$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1111331984296409</v>
       </c>
       <c r="O21" s="5">
-        <f>IF($A21=O$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>48</v>
+        <f>IF($A21=O$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.6666997976444613</v>
       </c>
       <c r="P21" s="5">
-        <f>IF($A21=P$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-2</v>
+        <f>IF($A21=P$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-6.9445824901852471E-2</v>
       </c>
       <c r="Q21" s="5">
-        <f>IF($A21=Q$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-12</v>
+        <f>IF($A21=Q$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.41667494941111527</v>
       </c>
       <c r="R21" s="5">
-        <f>IF($A21=R$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>2</v>
+        <f>IF($A21=R$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>6.9445824901852582E-2</v>
       </c>
       <c r="S21" s="5">
-        <f>IF($A21=S$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>87</v>
+        <f>IF($A21=S$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.020893383230586</v>
       </c>
       <c r="T21" s="5">
-        <f>IF($A21=T$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>64</v>
+        <f>IF($A21=T$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.2222663968592817</v>
       </c>
       <c r="U21" s="5">
-        <f>IF($A21=U$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>99</v>
+        <f>IF($A21=U$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.69287993481621069</v>
       </c>
       <c r="V21" s="5">
-        <f>IF($A21=V$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A21=V$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="W21" s="5">
-        <f>IF($A21=W$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>29</v>
+        <f>IF($A21=W$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.006964461076862</v>
       </c>
       <c r="X21" s="5">
-        <f>IF($A21=X$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>19.954545454545453</v>
+        <f>IF($A21=X$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.69287993481621069</v>
       </c>
       <c r="Y21" s="5">
-        <f>IF($A21=Y$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-28</v>
+        <f>IF($A21=Y$1,VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A21,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.9722415486259357</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
@@ -26794,100 +26891,100 @@
         <v>20</v>
       </c>
       <c r="B22" s="5">
-        <f>IF($A22=B$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A22=B$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
       <c r="C22" s="5">
-        <f>IF($A22=C$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A22=C$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="D22" s="5">
-        <f>IF($A22=D$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A22=D$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="E22" s="5">
-        <f>IF($A22=E$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A22=E$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="F22" s="5">
-        <f>IF($A22=F$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-11</v>
+        <f>IF($A22=F$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.38195203696018898</v>
       </c>
       <c r="G22" s="5">
-        <f>IF($A22=G$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A22=G$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="H22" s="5">
-        <f>IF($A22=H$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A22=H$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="I22" s="5">
-        <f>IF($A22=I$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A22=I$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027975</v>
       </c>
       <c r="J22" s="5">
-        <f>IF($A22=J$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>23</v>
+        <f>IF($A22=J$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.79862698637130436</v>
       </c>
       <c r="K22" s="5">
-        <f>IF($A22=K$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A22=K$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926263E-2</v>
       </c>
       <c r="L22" s="5">
-        <f>IF($A22=L$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-1</v>
+        <f>IF($A22=L$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-3.4722912450926263E-2</v>
       </c>
       <c r="M22" s="5">
-        <f>IF($A22=M$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>15</v>
+        <f>IF($A22=M$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.52084368676389414</v>
       </c>
       <c r="N22" s="5">
-        <f>IF($A22=N$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>17</v>
+        <f>IF($A22=N$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.59028951166574672</v>
       </c>
       <c r="O22" s="5">
-        <f>IF($A22=O$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>33</v>
+        <f>IF($A22=O$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1458561108805672</v>
       </c>
       <c r="P22" s="5">
-        <f>IF($A22=P$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-17</v>
+        <f>IF($A22=P$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.59028951166574661</v>
       </c>
       <c r="Q22" s="5">
-        <f>IF($A22=Q$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-27</v>
+        <f>IF($A22=Q$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.93751863617500941</v>
       </c>
       <c r="R22" s="5">
-        <f>IF($A22=R$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-13</v>
+        <f>IF($A22=R$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.45139786186204156</v>
       </c>
       <c r="S22" s="5">
-        <f>IF($A22=S$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>72</v>
+        <f>IF($A22=S$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.5000496964666916</v>
       </c>
       <c r="T22" s="5">
-        <f>IF($A22=T$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>49</v>
+        <f>IF($A22=T$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.7014227100953876</v>
       </c>
       <c r="U22" s="5">
-        <f>IF($A22=U$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A22=U$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="V22" s="5">
-        <f>IF($A22=V$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>114</v>
+        <f>IF($A22=V$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.17203624805231651</v>
       </c>
       <c r="W22" s="5">
-        <f>IF($A22=W$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>14</v>
+        <f>IF($A22=W$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.48612077431296785</v>
       </c>
       <c r="X22" s="5">
-        <f>IF($A22=X$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>4.9545454545454533</v>
+        <f>IF($A22=X$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.17203624805231651</v>
       </c>
       <c r="Y22" s="5">
-        <f>IF($A22=Y$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-43</v>
+        <f>IF($A22=Y$1,VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A22,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4930852353898298</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
@@ -26895,100 +26992,100 @@
         <v>21</v>
       </c>
       <c r="B23" s="5">
-        <f>IF($A23=B$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A23=B$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027977</v>
       </c>
       <c r="C23" s="5">
-        <f>IF($A23=C$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>29</v>
+        <f>IF($A23=C$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.006964461076862</v>
       </c>
       <c r="D23" s="5">
-        <f>IF($A23=D$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A23=D$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="E23" s="5">
-        <f>IF($A23=E$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A23=E$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="F23" s="5">
-        <f>IF($A23=F$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-25</v>
+        <f>IF($A23=F$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.86807281127315683</v>
       </c>
       <c r="G23" s="5">
-        <f>IF($A23=G$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A23=G$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="H23" s="5">
-        <f>IF($A23=H$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A23=H$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="I23" s="5">
-        <f>IF($A23=I$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-71</v>
+        <f>IF($A23=I$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.4653267840157653</v>
       </c>
       <c r="J23" s="5">
-        <f>IF($A23=J$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>9</v>
+        <f>IF($A23=J$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31250621205833645</v>
       </c>
       <c r="K23" s="5">
-        <f>IF($A23=K$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A23=K$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="L23" s="5">
-        <f>IF($A23=L$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15</v>
+        <f>IF($A23=L$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.52084368676389414</v>
       </c>
       <c r="M23" s="5">
-        <f>IF($A23=M$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>1</v>
+        <f>IF($A23=M$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.4722912450926291E-2</v>
       </c>
       <c r="N23" s="5">
-        <f>IF($A23=N$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>3</v>
+        <f>IF($A23=N$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.10416873735277882</v>
       </c>
       <c r="O23" s="5">
-        <f>IF($A23=O$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>19</v>
+        <f>IF($A23=O$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.65973533656759931</v>
       </c>
       <c r="P23" s="5">
-        <f>IF($A23=P$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-31</v>
+        <f>IF($A23=P$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.0764102859787146</v>
       </c>
       <c r="Q23" s="5">
-        <f>IF($A23=Q$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-41</v>
+        <f>IF($A23=Q$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.4236394104879773</v>
       </c>
       <c r="R23" s="5">
-        <f>IF($A23=R$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-27</v>
+        <f>IF($A23=R$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.93751863617500941</v>
       </c>
       <c r="S23" s="5">
-        <f>IF($A23=S$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>58</v>
+        <f>IF($A23=S$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.013928922153724</v>
       </c>
       <c r="T23" s="5">
-        <f>IF($A23=T$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>35</v>
+        <f>IF($A23=T$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.2153019357824197</v>
       </c>
       <c r="U23" s="5">
-        <f>IF($A23=U$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-29</v>
+        <f>IF($A23=U$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.006964461076862</v>
       </c>
       <c r="V23" s="5">
-        <f>IF($A23=V$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A23=V$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296785</v>
       </c>
       <c r="W23" s="5">
-        <f>IF($A23=W$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>128</v>
+        <f>IF($A23=W$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31408452626065136</v>
       </c>
       <c r="X23" s="5">
-        <f>IF($A23=X$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-9.0454545454545467</v>
+        <f>IF($A23=X$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.31408452626065136</v>
       </c>
       <c r="Y23" s="5">
-        <f>IF($A23=Y$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-57</v>
+        <f>IF($A23=Y$1,VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A23,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.9792060097027977</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -26996,100 +27093,100 @@
         <v>22</v>
       </c>
       <c r="B24" s="5">
-        <f>IF($A24=B$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-47.954545454545453</v>
+        <f>IF($A24=B$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.6651214834421464</v>
       </c>
       <c r="C24" s="5">
-        <f>IF($A24=C$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>38.045454545454547</v>
+        <f>IF($A24=C$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.3210489873375133</v>
       </c>
       <c r="D24" s="5">
-        <f>IF($A24=D$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-4.9545454545454533</v>
+        <f>IF($A24=D$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.17203624805231651</v>
       </c>
       <c r="E24" s="5">
-        <f>IF($A24=E$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-4.9545454545454533</v>
+        <f>IF($A24=E$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.17203624805231651</v>
       </c>
       <c r="F24" s="5">
-        <f>IF($A24=F$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-15.954545454545453</v>
+        <f>IF($A24=F$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.55398828501250552</v>
       </c>
       <c r="G24" s="5">
-        <f>IF($A24=G$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>9.0454545454545467</v>
+        <f>IF($A24=G$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31408452626065136</v>
       </c>
       <c r="H24" s="5">
-        <f>IF($A24=H$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>9.0454545454545467</v>
+        <f>IF($A24=H$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31408452626065136</v>
       </c>
       <c r="I24" s="5">
-        <f>IF($A24=I$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-61.954545454545453</v>
+        <f>IF($A24=I$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-2.151242257755114</v>
       </c>
       <c r="J24" s="5">
-        <f>IF($A24=J$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>18.045454545454547</v>
+        <f>IF($A24=J$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.62659073831898782</v>
       </c>
       <c r="K24" s="5">
-        <f>IF($A24=K$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-5.9545454545454533</v>
+        <f>IF($A24=K$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.20675916050324278</v>
       </c>
       <c r="L24" s="5">
-        <f>IF($A24=L$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-5.9545454545454533</v>
+        <f>IF($A24=L$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.20675916050324278</v>
       </c>
       <c r="M24" s="5">
-        <f>IF($A24=M$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>10.045454545454547</v>
+        <f>IF($A24=M$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.34880743871157766</v>
       </c>
       <c r="N24" s="5">
-        <f>IF($A24=N$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>12.045454545454547</v>
+        <f>IF($A24=N$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.41825326361343018</v>
       </c>
       <c r="O24" s="5">
-        <f>IF($A24=O$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>28.045454545454547</v>
+        <f>IF($A24=O$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.97381986282825062</v>
       </c>
       <c r="P24" s="5">
-        <f>IF($A24=P$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-21.954545454545453</v>
+        <f>IF($A24=P$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.76232575971806316</v>
       </c>
       <c r="Q24" s="5">
-        <f>IF($A24=Q$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-31.954545454545453</v>
+        <f>IF($A24=Q$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.109554884227326</v>
       </c>
       <c r="R24" s="5">
-        <f>IF($A24=R$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-17.954545454545453</v>
+        <f>IF($A24=R$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.6234341099143581</v>
       </c>
       <c r="S24" s="5">
-        <f>IF($A24=S$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>67.045454545454547</v>
+        <f>IF($A24=S$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.3280134484143753</v>
       </c>
       <c r="T24" s="5">
-        <f>IF($A24=T$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>44.045454545454547</v>
+        <f>IF($A24=T$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.529386462043071</v>
       </c>
       <c r="U24" s="5">
-        <f>IF($A24=U$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-19.954545454545453</v>
+        <f>IF($A24=U$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.69287993481621069</v>
       </c>
       <c r="V24" s="5">
-        <f>IF($A24=V$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-4.9545454545454533</v>
+        <f>IF($A24=V$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.17203624805231651</v>
       </c>
       <c r="W24" s="5">
-        <f>IF($A24=W$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>9.0454545454545467</v>
+        <f>IF($A24=W$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.31408452626065136</v>
       </c>
       <c r="X24" s="5">
-        <f>IF($A24=X$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>118.95454545454545</v>
+        <f>IF($A24=X$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0</v>
       </c>
       <c r="Y24" s="5">
-        <f>IF($A24=Y$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-47.954545454545453</v>
+        <f>IF($A24=Y$1,VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A24,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.6651214834421464</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -27097,100 +27194,100 @@
         <v>23</v>
       </c>
       <c r="B25" s="5">
-        <f>IF($A25=B$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
+        <f>IF($A25=B$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(B$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
         <v>0</v>
       </c>
       <c r="C25" s="5">
-        <f>IF($A25=C$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>86</v>
+        <f>IF($A25=C$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(C$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.9861704707796597</v>
       </c>
       <c r="D25" s="5">
-        <f>IF($A25=D$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A25=D$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(D$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="E25" s="5">
-        <f>IF($A25=E$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A25=E$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(E$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="F25" s="5">
-        <f>IF($A25=F$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>32</v>
+        <f>IF($A25=F$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(F$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.1111331984296409</v>
       </c>
       <c r="G25" s="5">
-        <f>IF($A25=G$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A25=G$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(G$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027977</v>
       </c>
       <c r="H25" s="5">
-        <f>IF($A25=H$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A25=H$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(H$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027977</v>
       </c>
       <c r="I25" s="5">
-        <f>IF($A25=I$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>-14</v>
+        <f>IF($A25=I$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(I$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-0.48612077431296763</v>
       </c>
       <c r="J25" s="5">
-        <f>IF($A25=J$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>66</v>
+        <f>IF($A25=J$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(J$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.2917122217611343</v>
       </c>
       <c r="K25" s="5">
-        <f>IF($A25=K$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>42</v>
+        <f>IF($A25=K$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(K$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4583623229389036</v>
       </c>
       <c r="L25" s="5">
-        <f>IF($A25=L$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>42</v>
+        <f>IF($A25=L$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(L$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4583623229389036</v>
       </c>
       <c r="M25" s="5">
-        <f>IF($A25=M$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>58</v>
+        <f>IF($A25=M$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(M$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.013928922153724</v>
       </c>
       <c r="N25" s="5">
-        <f>IF($A25=N$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>60</v>
+        <f>IF($A25=N$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(N$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.0833747470555766</v>
       </c>
       <c r="O25" s="5">
-        <f>IF($A25=O$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>76</v>
+        <f>IF($A25=O$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(O$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>2.6389413462703972</v>
       </c>
       <c r="P25" s="5">
-        <f>IF($A25=P$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>26</v>
+        <f>IF($A25=P$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(P$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.90279572372408323</v>
       </c>
       <c r="Q25" s="5">
-        <f>IF($A25=Q$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>16</v>
+        <f>IF($A25=Q$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Q$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.55556659921482043</v>
       </c>
       <c r="R25" s="5">
-        <f>IF($A25=R$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>30</v>
+        <f>IF($A25=R$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(R$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.0416873735277883</v>
       </c>
       <c r="S25" s="5">
-        <f>IF($A25=S$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>115</v>
+        <f>IF($A25=S$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(S$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.9931349318565217</v>
       </c>
       <c r="T25" s="5">
-        <f>IF($A25=T$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>92</v>
+        <f>IF($A25=T$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(T$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>3.1945079454852174</v>
       </c>
       <c r="U25" s="5">
-        <f>IF($A25=U$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>28</v>
+        <f>IF($A25=U$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(U$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>0.9722415486259357</v>
       </c>
       <c r="V25" s="5">
-        <f>IF($A25=V$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>43</v>
+        <f>IF($A25=V$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(V$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.4930852353898298</v>
       </c>
       <c r="W25" s="5">
-        <f>IF($A25=W$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>57</v>
+        <f>IF($A25=W$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(W$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.9792060097027977</v>
       </c>
       <c r="X25" s="5">
-        <f>IF($A25=X$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>47.954545454545453</v>
+        <f>IF($A25=X$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(X$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>1.6651214834421464</v>
       </c>
       <c r="Y25" s="5">
-        <f>IF($A25=Y$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,2,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,2,0))</f>
-        <v>71</v>
+        <f>IF($A25=Y$1,VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0),VLOOKUP(Y$1,'Size Lookup'!$A$2:$G$25,3,0)-VLOOKUP($A25,'Size Lookup'!$A$2:$G$25,3,0))</f>
+        <v>-1.6651214834421464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated MULTIPLE/SIZE scheme with rescaled values
</commit_message>
<xml_diff>
--- a/encoding_schemes.xlsx
+++ b/encoding_schemes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxc533/Documents/Arbejde/PhD/Kurser/Kursusmapper/Algorithms_in_Bioinformatics/Exercises/Algo/Algo2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E350824-ECC3-6040-91E6-F814C5358E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0FA4CE-7413-384C-9A63-BA356D1B5E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" firstSheet="8" activeTab="8" xr2:uid="{3BD1CE7E-F90B-5740-A5D3-7EC0EBF1FABD}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="52">
   <si>
     <t>A</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>Scaled</t>
+  </si>
+  <si>
+    <t>Soruce:</t>
+  </si>
+  <si>
+    <t>https://www.chem.ucalgary.ca/courses/351/Carey5th/Ch27/ch27-1-4-2.html</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -6051,10 +6060,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549A4F79-BC58-1F4E-9FFB-47F04CA66FF8}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6725,6 +6734,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6735,7 +6752,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7147,7 +7164,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
         <v>45</v>
       </c>
     </row>
@@ -24775,7 +24795,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>